<commit_message>
TMA: Release Atom and E-Core updates
Release CSV and XSLX formats for Atom and E-Core TMA. XLSX change log
notes copied below.

- Atom TMA version 1.1.
    - FP_UOPS changed to FPDIV_Uops
    - Added BR_MISP breakdown stats
    - Frontend_Bandwidth/Latency changed to Fetch_Bandwidth/Latency
    - Load_Store_Bound changed to Memory_Bound
    - Icache changed to ICache_Misses
    - ITLB changed to ITLB_Misses

- E-Core TMA version 2.3.
    - FP_UOPS changed to FPDIV_Uops
    - Added BR_MISP breakdown stats
    - Frontend_Bandwidth/Latency changed to Fetch_Bandwidth/Latency
    - Load_Store_Bound changed to Memory_Bound
    - Icache changed to ICache_Misses
    - ITLB changed to ITLB_Misses
    - Store_Fwd changed to Store_Fwd_Blk
</commit_message>
<xml_diff>
--- a/Atom_TMA.xlsx
+++ b/Atom_TMA.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15990" tabRatio="575" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="575" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Change Log" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="32">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -219,8 +219,27 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FFC00000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="-apple-system"/>
       <color theme="1"/>
-      <sz val="9"/>
+      <sz val="10.5"/>
     </font>
   </fonts>
   <fills count="54">
@@ -786,7 +805,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -851,9 +870,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="53" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="53" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="53" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -868,7 +884,20 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="34" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -881,7 +910,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -900,7 +928,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1268,7 +1300,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1287,8 +1319,8 @@
           <t>Version</t>
         </is>
       </c>
-      <c r="C1" s="53" t="n">
-        <v>1</v>
+      <c r="C1" s="3" t="n">
+        <v>1.1</v>
       </c>
     </row>
     <row r="2">
@@ -1299,62 +1331,62 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="54" t="inlineStr">
+      <c r="A3" s="58" t="inlineStr">
         <is>
           <t>Key</t>
         </is>
       </c>
-      <c r="B3" s="54" t="inlineStr">
+      <c r="B3" s="58" t="inlineStr">
         <is>
           <t>Level1</t>
         </is>
       </c>
-      <c r="C3" s="54" t="inlineStr">
+      <c r="C3" s="58" t="inlineStr">
         <is>
           <t>Level2</t>
         </is>
       </c>
-      <c r="D3" s="54" t="inlineStr">
+      <c r="D3" s="58" t="inlineStr">
         <is>
           <t>Level3</t>
         </is>
       </c>
-      <c r="E3" s="54" t="inlineStr">
+      <c r="E3" s="58" t="inlineStr">
         <is>
           <t>Level4</t>
         </is>
       </c>
-      <c r="F3" s="54" t="inlineStr">
+      <c r="F3" s="58" t="inlineStr">
         <is>
           <t>TNT</t>
         </is>
       </c>
-      <c r="G3" s="54" t="inlineStr">
+      <c r="G3" s="58" t="inlineStr">
         <is>
           <t>GLM/GLP</t>
         </is>
       </c>
-      <c r="H3" s="54" t="inlineStr">
+      <c r="H3" s="58" t="inlineStr">
         <is>
           <t>Locate-with</t>
         </is>
       </c>
-      <c r="I3" s="54" t="inlineStr">
+      <c r="I3" s="58" t="inlineStr">
         <is>
           <t>Count Domain</t>
         </is>
       </c>
-      <c r="J3" s="54" t="inlineStr">
+      <c r="J3" s="58" t="inlineStr">
         <is>
           <t>Metric Description</t>
         </is>
       </c>
-      <c r="K3" s="54" t="inlineStr">
+      <c r="K3" s="58" t="inlineStr">
         <is>
           <t>Metric Group</t>
         </is>
       </c>
-      <c r="L3" s="54" t="inlineStr">
+      <c r="L3" s="58" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
@@ -1366,7 +1398,7 @@
           <t>FE</t>
         </is>
       </c>
-      <c r="B4" s="55" t="inlineStr">
+      <c r="B4" s="59" t="inlineStr">
         <is>
           <t>Frontend_Bound</t>
         </is>
@@ -1374,18 +1406,18 @@
       <c r="C4" s="24" t="n"/>
       <c r="D4" s="24" t="n"/>
       <c r="E4" s="8" t="n"/>
-      <c r="F4" s="44" t="inlineStr">
+      <c r="F4" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.ALL / SLOTS</t>
         </is>
       </c>
-      <c r="G4" s="44" t="inlineStr">
+      <c r="G4" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">UOPS_NOT_DELIVERED.ANY / SLOTS </t>
         </is>
       </c>
-      <c r="H4" s="44" t="n"/>
-      <c r="I4" s="44" t="inlineStr">
+      <c r="H4" s="7" t="n"/>
+      <c r="I4" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1409,21 +1441,21 @@
         </is>
       </c>
       <c r="B5" s="24" t="n"/>
-      <c r="C5" s="56" t="inlineStr">
-        <is>
-          <t>Frontend_Latency</t>
+      <c r="C5" s="60" t="inlineStr">
+        <is>
+          <t>Fetch_Latency</t>
         </is>
       </c>
       <c r="D5" s="24" t="n"/>
       <c r="E5" s="8" t="n"/>
-      <c r="F5" s="44" t="inlineStr">
+      <c r="F5" s="7" t="inlineStr">
         <is>
           <t>( TOPDOWN_FE_BOUND.ITLB + TOPDOWN_FE_BOUND.ICACHE + TOPDOWN_FE_BOUND.BRANCH_DETECT +  TOPDOWN_FE_BOUND.BRANCH_RESTEER ) / SLOTS</t>
         </is>
       </c>
-      <c r="G5" s="44" t="n"/>
-      <c r="H5" s="44" t="n"/>
-      <c r="I5" s="44" t="inlineStr">
+      <c r="G5" s="7" t="n"/>
+      <c r="H5" s="7" t="n"/>
+      <c r="I5" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1448,20 +1480,20 @@
       </c>
       <c r="B6" s="24" t="n"/>
       <c r="C6" s="24" t="n"/>
-      <c r="D6" s="57" t="inlineStr">
-        <is>
-          <t>Icache</t>
+      <c r="D6" s="61" t="inlineStr">
+        <is>
+          <t>ICache_Misses</t>
         </is>
       </c>
       <c r="E6" s="8" t="n"/>
-      <c r="F6" s="44" t="inlineStr">
+      <c r="F6" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.ICACHE / SLOTS</t>
         </is>
       </c>
-      <c r="G6" s="44" t="n"/>
-      <c r="H6" s="44" t="n"/>
-      <c r="I6" s="44" t="inlineStr">
+      <c r="G6" s="7" t="n"/>
+      <c r="H6" s="7" t="n"/>
+      <c r="I6" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1486,20 +1518,20 @@
       </c>
       <c r="B7" s="24" t="n"/>
       <c r="C7" s="24" t="n"/>
-      <c r="D7" s="57" t="inlineStr">
-        <is>
-          <t>ITLB</t>
+      <c r="D7" s="61" t="inlineStr">
+        <is>
+          <t>ITLB_Misses</t>
         </is>
       </c>
       <c r="E7" s="8" t="n"/>
-      <c r="F7" s="44" t="inlineStr">
+      <c r="F7" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.ITLB / SLOTS</t>
         </is>
       </c>
-      <c r="G7" s="44" t="n"/>
-      <c r="H7" s="44" t="n"/>
-      <c r="I7" s="44" t="inlineStr">
+      <c r="G7" s="7" t="n"/>
+      <c r="H7" s="7" t="n"/>
+      <c r="I7" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1524,20 +1556,20 @@
       </c>
       <c r="B8" s="24" t="n"/>
       <c r="C8" s="24" t="n"/>
-      <c r="D8" s="57" t="inlineStr">
+      <c r="D8" s="61" t="inlineStr">
         <is>
           <t>Branch_Detect</t>
         </is>
       </c>
       <c r="E8" s="8" t="n"/>
-      <c r="F8" s="44" t="inlineStr">
+      <c r="F8" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.BRANCH_DETECT / SLOTS</t>
         </is>
       </c>
-      <c r="G8" s="44" t="n"/>
-      <c r="H8" s="44" t="n"/>
-      <c r="I8" s="44" t="inlineStr">
+      <c r="G8" s="7" t="n"/>
+      <c r="H8" s="7" t="n"/>
+      <c r="I8" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1562,20 +1594,20 @@
       </c>
       <c r="B9" s="24" t="n"/>
       <c r="C9" s="24" t="n"/>
-      <c r="D9" s="57" t="inlineStr">
+      <c r="D9" s="61" t="inlineStr">
         <is>
           <t>Branch_Resteer</t>
         </is>
       </c>
       <c r="E9" s="8" t="n"/>
-      <c r="F9" s="44" t="inlineStr">
+      <c r="F9" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.BRANCH_RESTEER / SLOTS</t>
         </is>
       </c>
-      <c r="G9" s="44" t="n"/>
-      <c r="H9" s="44" t="n"/>
-      <c r="I9" s="44" t="inlineStr">
+      <c r="G9" s="7" t="n"/>
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1599,21 +1631,21 @@
         </is>
       </c>
       <c r="B10" s="24" t="n"/>
-      <c r="C10" s="56" t="inlineStr">
-        <is>
-          <t>Frontend_Bandwidth</t>
+      <c r="C10" s="60" t="inlineStr">
+        <is>
+          <t>Fetch_Bandwidth</t>
         </is>
       </c>
       <c r="D10" s="24" t="n"/>
       <c r="E10" s="8" t="n"/>
-      <c r="F10" s="44" t="inlineStr">
+      <c r="F10" s="7" t="inlineStr">
         <is>
           <t>( TOPDOWN_FE_BOUND.CISC + TOPDOWN_FE_BOUND.DECODE + TOPDOWN_FE_BOUND.PREDECODE + TOPDOWN_FE_BOUND.OTHER ) / SLOTS</t>
         </is>
       </c>
-      <c r="G10" s="44" t="n"/>
-      <c r="H10" s="44" t="n"/>
-      <c r="I10" s="44" t="inlineStr">
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="7" t="n"/>
+      <c r="I10" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1638,20 +1670,20 @@
       </c>
       <c r="B11" s="24" t="n"/>
       <c r="C11" s="24" t="n"/>
-      <c r="D11" s="57" t="inlineStr">
+      <c r="D11" s="61" t="inlineStr">
         <is>
           <t>Cisc</t>
         </is>
       </c>
       <c r="E11" s="8" t="n"/>
-      <c r="F11" s="44" t="inlineStr">
+      <c r="F11" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.CISC / SLOTS</t>
         </is>
       </c>
-      <c r="G11" s="44" t="n"/>
-      <c r="H11" s="44" t="n"/>
-      <c r="I11" s="44" t="inlineStr">
+      <c r="G11" s="7" t="n"/>
+      <c r="H11" s="7" t="n"/>
+      <c r="I11" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1676,20 +1708,20 @@
       </c>
       <c r="B12" s="24" t="n"/>
       <c r="C12" s="24" t="n"/>
-      <c r="D12" s="57" t="inlineStr">
+      <c r="D12" s="61" t="inlineStr">
         <is>
           <t>Decode</t>
         </is>
       </c>
       <c r="E12" s="8" t="n"/>
-      <c r="F12" s="44" t="inlineStr">
+      <c r="F12" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.DECODE / SLOTS</t>
         </is>
       </c>
-      <c r="G12" s="44" t="n"/>
-      <c r="H12" s="44" t="n"/>
-      <c r="I12" s="44" t="inlineStr">
+      <c r="G12" s="7" t="n"/>
+      <c r="H12" s="7" t="n"/>
+      <c r="I12" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1714,20 +1746,20 @@
       </c>
       <c r="B13" s="24" t="n"/>
       <c r="C13" s="24" t="n"/>
-      <c r="D13" s="57" t="inlineStr">
+      <c r="D13" s="61" t="inlineStr">
         <is>
           <t>Predecode</t>
         </is>
       </c>
       <c r="E13" s="8" t="n"/>
-      <c r="F13" s="44" t="inlineStr">
+      <c r="F13" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.PREDECODE / SLOTS</t>
         </is>
       </c>
-      <c r="G13" s="44" t="n"/>
-      <c r="H13" s="44" t="n"/>
-      <c r="I13" s="44" t="inlineStr">
+      <c r="G13" s="7" t="n"/>
+      <c r="H13" s="7" t="n"/>
+      <c r="I13" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1752,20 +1784,20 @@
       </c>
       <c r="B14" s="24" t="n"/>
       <c r="C14" s="24" t="n"/>
-      <c r="D14" s="57" t="inlineStr">
+      <c r="D14" s="61" t="inlineStr">
         <is>
           <t>Other_FB</t>
         </is>
       </c>
       <c r="E14" s="8" t="n"/>
-      <c r="F14" s="44" t="inlineStr">
+      <c r="F14" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_FE_BOUND.OTHER / SLOTS</t>
         </is>
       </c>
-      <c r="G14" s="44" t="n"/>
-      <c r="H14" s="44" t="n"/>
-      <c r="I14" s="44" t="inlineStr">
+      <c r="G14" s="7" t="n"/>
+      <c r="H14" s="7" t="n"/>
+      <c r="I14" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1788,26 +1820,26 @@
           <t>BAD</t>
         </is>
       </c>
-      <c r="B15" s="58" t="inlineStr">
+      <c r="B15" s="62" t="inlineStr">
         <is>
           <t>Bad_Speculation</t>
         </is>
       </c>
-      <c r="C15" s="59" t="n"/>
-      <c r="D15" s="59" t="n"/>
+      <c r="C15" s="63" t="n"/>
+      <c r="D15" s="63" t="n"/>
       <c r="E15" s="8" t="n"/>
-      <c r="F15" s="44" t="inlineStr">
+      <c r="F15" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BAD_SPECULATION.ALL / SLOTS</t>
         </is>
       </c>
-      <c r="G15" s="44" t="inlineStr">
+      <c r="G15" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">( UOPS_ISSUED.ANY - UOPS_RETIRED.ANY +  ISSUE_SLOTS_NOT_CONSUMED.RECOVERY )  / SLOTS </t>
         </is>
       </c>
-      <c r="H15" s="44" t="n"/>
-      <c r="I15" s="44" t="inlineStr">
+      <c r="H15" s="7" t="n"/>
+      <c r="I15" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1830,22 +1862,22 @@
           <t>BAD</t>
         </is>
       </c>
-      <c r="B16" s="59" t="n"/>
-      <c r="C16" s="60" t="inlineStr">
+      <c r="B16" s="63" t="n"/>
+      <c r="C16" s="64" t="inlineStr">
         <is>
           <t>Branch_Mispredicts</t>
         </is>
       </c>
-      <c r="D16" s="59" t="n"/>
+      <c r="D16" s="63" t="n"/>
       <c r="E16" s="8" t="n"/>
-      <c r="F16" s="44" t="inlineStr">
+      <c r="F16" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BAD_SPECULATION.MISPREDICT / SLOTS</t>
         </is>
       </c>
-      <c r="G16" s="44" t="n"/>
-      <c r="H16" s="44" t="n"/>
-      <c r="I16" s="44" t="inlineStr">
+      <c r="G16" s="7" t="n"/>
+      <c r="H16" s="7" t="n"/>
+      <c r="I16" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1868,22 +1900,22 @@
           <t>BAD</t>
         </is>
       </c>
-      <c r="B17" s="61" t="n"/>
-      <c r="C17" s="60" t="inlineStr">
+      <c r="B17" s="65" t="n"/>
+      <c r="C17" s="64" t="inlineStr">
         <is>
           <t>Machine_Clears</t>
         </is>
       </c>
-      <c r="D17" s="59" t="n"/>
+      <c r="D17" s="63" t="n"/>
       <c r="E17" s="8" t="n"/>
-      <c r="F17" s="44" t="inlineStr">
+      <c r="F17" s="7" t="inlineStr">
         <is>
           <t>( TOPDOWN_BAD_SPECULATION.MONUKE ) / SLOTS</t>
         </is>
       </c>
-      <c r="G17" s="44" t="n"/>
-      <c r="H17" s="44" t="n"/>
-      <c r="I17" s="44" t="inlineStr">
+      <c r="G17" s="7" t="n"/>
+      <c r="H17" s="7" t="n"/>
+      <c r="I17" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1906,22 +1938,22 @@
           <t>BAD</t>
         </is>
       </c>
-      <c r="B18" s="59" t="n"/>
-      <c r="C18" s="59" t="n"/>
-      <c r="D18" s="62" t="inlineStr">
+      <c r="B18" s="63" t="n"/>
+      <c r="C18" s="63" t="n"/>
+      <c r="D18" s="66" t="inlineStr">
         <is>
           <t>Fast_Nuke</t>
         </is>
       </c>
       <c r="E18" s="8" t="n"/>
-      <c r="F18" s="44" t="inlineStr">
+      <c r="F18" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BAD_SPECULATION.MONUKE / SLOTS</t>
         </is>
       </c>
-      <c r="G18" s="44" t="n"/>
-      <c r="H18" s="44" t="n"/>
-      <c r="I18" s="44" t="inlineStr">
+      <c r="G18" s="7" t="n"/>
+      <c r="H18" s="7" t="n"/>
+      <c r="I18" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1944,26 +1976,26 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B19" s="63" t="inlineStr">
+      <c r="B19" s="67" t="inlineStr">
         <is>
           <t>Backend_Bound</t>
         </is>
       </c>
-      <c r="C19" s="64" t="n"/>
-      <c r="D19" s="64" t="n"/>
+      <c r="C19" s="57" t="n"/>
+      <c r="D19" s="57" t="n"/>
       <c r="E19" s="8" t="n"/>
-      <c r="F19" s="44" t="inlineStr">
+      <c r="F19" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BE_BOUND.ALL / SLOTS</t>
         </is>
       </c>
-      <c r="G19" s="44" t="inlineStr">
+      <c r="G19" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">ISSUE_SLOTS_NOT_CONSUMED.RESOURCE_FULL / SLOTS </t>
         </is>
       </c>
-      <c r="H19" s="44" t="n"/>
-      <c r="I19" s="44" t="inlineStr">
+      <c r="H19" s="7" t="n"/>
+      <c r="I19" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -1986,21 +2018,21 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B20" s="65" t="n"/>
-      <c r="C20" s="66" t="inlineStr">
+      <c r="B20" s="68" t="n"/>
+      <c r="C20" s="69" t="inlineStr">
         <is>
           <t>Core_Bound</t>
         </is>
       </c>
       <c r="E20" s="8" t="n"/>
-      <c r="F20" s="44" t="inlineStr">
-        <is>
-          <t>max( 0 , Backend_Bound - Load_Store_Bound )</t>
-        </is>
-      </c>
-      <c r="G20" s="44" t="n"/>
-      <c r="H20" s="44" t="n"/>
-      <c r="I20" s="44" t="inlineStr">
+      <c r="F20" s="7" t="inlineStr">
+        <is>
+          <t>max( 0 , Backend_Bound - Memory_Bound )</t>
+        </is>
+      </c>
+      <c r="G20" s="7" t="n"/>
+      <c r="H20" s="7" t="n"/>
+      <c r="I20" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2023,22 +2055,22 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B21" s="65" t="n"/>
-      <c r="C21" s="66" t="inlineStr">
-        <is>
-          <t>Load_Store_Bound</t>
-        </is>
-      </c>
-      <c r="D21" s="64" t="n"/>
+      <c r="B21" s="68" t="n"/>
+      <c r="C21" s="69" t="inlineStr">
+        <is>
+          <t>Memory_Bound</t>
+        </is>
+      </c>
+      <c r="D21" s="57" t="n"/>
       <c r="E21" s="8" t="n"/>
-      <c r="F21" s="44" t="inlineStr">
+      <c r="F21" s="7" t="inlineStr">
         <is>
           <t>( MEM_BOUND_STALLS.LOAD_L2_HIT + MEM_BOUND_STALLS.LOAD_LLC_HIT + MEM_BOUND_STALLS.LOAD_DRAM_HIT+ MEM_BOUND_STALLS.STORE_BUFFER_FULL) / CLKS</t>
         </is>
       </c>
-      <c r="G21" s="44" t="n"/>
-      <c r="H21" s="44" t="n"/>
-      <c r="I21" s="44" t="inlineStr">
+      <c r="G21" s="7" t="n"/>
+      <c r="H21" s="7" t="n"/>
+      <c r="I21" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2061,22 +2093,22 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B22" s="64" t="n"/>
-      <c r="C22" s="64" t="n"/>
-      <c r="D22" s="67" t="inlineStr">
+      <c r="B22" s="57" t="n"/>
+      <c r="C22" s="57" t="n"/>
+      <c r="D22" s="70" t="inlineStr">
         <is>
           <t>Store_Bound</t>
         </is>
       </c>
       <c r="E22" s="22" t="n"/>
-      <c r="F22" s="44" t="inlineStr">
+      <c r="F22" s="7" t="inlineStr">
         <is>
           <t>MEM_BOUND_STALLS.STORE_BUFFER_FULL / CLKS</t>
         </is>
       </c>
-      <c r="G22" s="44" t="n"/>
-      <c r="H22" s="44" t="n"/>
-      <c r="I22" s="44" t="inlineStr">
+      <c r="G22" s="7" t="n"/>
+      <c r="H22" s="7" t="n"/>
+      <c r="I22" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2099,20 +2131,20 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B23" s="61" t="n"/>
-      <c r="D23" s="68" t="inlineStr">
+      <c r="B23" s="65" t="n"/>
+      <c r="D23" s="71" t="inlineStr">
         <is>
           <t>L2_Bound</t>
         </is>
       </c>
-      <c r="F23" s="44" t="inlineStr">
+      <c r="F23" s="7" t="inlineStr">
         <is>
           <t>MEM_BOUND_STALLS.LOAD_L2_HIT / CLKS</t>
         </is>
       </c>
-      <c r="G23" s="44" t="n"/>
-      <c r="H23" s="44" t="n"/>
-      <c r="I23" s="44" t="inlineStr">
+      <c r="G23" s="7" t="n"/>
+      <c r="H23" s="7" t="n"/>
+      <c r="I23" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2135,20 +2167,20 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B24" s="64" t="n"/>
-      <c r="D24" s="68" t="inlineStr">
+      <c r="B24" s="57" t="n"/>
+      <c r="D24" s="71" t="inlineStr">
         <is>
           <t>L3_Bound</t>
         </is>
       </c>
-      <c r="F24" s="44" t="inlineStr">
+      <c r="F24" s="7" t="inlineStr">
         <is>
           <t>MEM_BOUND_STALLS.LOAD_LLC_HIT / CLKS</t>
         </is>
       </c>
-      <c r="G24" s="44" t="n"/>
-      <c r="H24" s="44" t="n"/>
-      <c r="I24" s="44" t="inlineStr">
+      <c r="G24" s="7" t="n"/>
+      <c r="H24" s="7" t="n"/>
+      <c r="I24" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2171,20 +2203,20 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B25" s="64" t="n"/>
+      <c r="B25" s="57" t="n"/>
       <c r="D25" s="38" t="inlineStr">
         <is>
           <t>DRAM_Bound</t>
         </is>
       </c>
-      <c r="F25" s="44" t="inlineStr">
+      <c r="F25" s="7" t="inlineStr">
         <is>
           <t>MEM_BOUND_STALLS.LOAD_DRAM_HIT / CLKS</t>
         </is>
       </c>
-      <c r="G25" s="44" t="n"/>
-      <c r="H25" s="44" t="n"/>
-      <c r="I25" s="44" t="inlineStr">
+      <c r="G25" s="7" t="n"/>
+      <c r="H25" s="7" t="n"/>
+      <c r="I25" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2207,26 +2239,26 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B26" s="69" t="inlineStr">
+      <c r="B26" s="72" t="inlineStr">
         <is>
           <t>Backend_Bound_Aux</t>
         </is>
       </c>
-      <c r="C26" s="59" t="n"/>
-      <c r="D26" s="59" t="n"/>
+      <c r="C26" s="63" t="n"/>
+      <c r="D26" s="63" t="n"/>
       <c r="E26" s="8" t="n"/>
-      <c r="F26" s="44" t="inlineStr">
+      <c r="F26" s="7" t="inlineStr">
         <is>
           <t>Backend_Bound</t>
         </is>
       </c>
-      <c r="G26" s="44" t="inlineStr">
+      <c r="G26" s="7" t="inlineStr">
         <is>
           <t>Backend_Bound</t>
         </is>
       </c>
-      <c r="H26" s="44" t="n"/>
-      <c r="I26" s="44" t="inlineStr">
+      <c r="H26" s="7" t="n"/>
+      <c r="I26" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2249,22 +2281,22 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B27" s="59" t="n"/>
-      <c r="C27" s="70" t="inlineStr">
+      <c r="B27" s="63" t="n"/>
+      <c r="C27" s="73" t="inlineStr">
         <is>
           <t>Resource_Bound</t>
         </is>
       </c>
-      <c r="D27" s="59" t="n"/>
+      <c r="D27" s="63" t="n"/>
       <c r="E27" s="8" t="n"/>
-      <c r="F27" s="44" t="inlineStr">
+      <c r="F27" s="7" t="inlineStr">
         <is>
           <t>Backend_Bound</t>
         </is>
       </c>
-      <c r="G27" s="44" t="n"/>
-      <c r="H27" s="44" t="n"/>
-      <c r="I27" s="44" t="inlineStr">
+      <c r="G27" s="7" t="n"/>
+      <c r="H27" s="7" t="n"/>
+      <c r="I27" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2287,22 +2319,22 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B28" s="59" t="n"/>
-      <c r="C28" s="59" t="n"/>
-      <c r="D28" s="71" t="inlineStr">
+      <c r="B28" s="63" t="n"/>
+      <c r="C28" s="63" t="n"/>
+      <c r="D28" s="74" t="inlineStr">
         <is>
           <t>Mem_Scheduler</t>
         </is>
       </c>
       <c r="E28" s="8" t="n"/>
-      <c r="F28" s="44" t="inlineStr">
+      <c r="F28" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BE_BOUND.MEM_SCHEDULER / SLOTS</t>
         </is>
       </c>
-      <c r="G28" s="44" t="n"/>
-      <c r="H28" s="44" t="n"/>
-      <c r="I28" s="44" t="inlineStr">
+      <c r="G28" s="7" t="n"/>
+      <c r="H28" s="7" t="n"/>
+      <c r="I28" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2325,22 +2357,22 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B29" s="59" t="n"/>
-      <c r="C29" s="59" t="n"/>
-      <c r="D29" s="71" t="inlineStr">
+      <c r="B29" s="63" t="n"/>
+      <c r="C29" s="63" t="n"/>
+      <c r="D29" s="74" t="inlineStr">
         <is>
           <t>Non_Mem_Scheduler</t>
         </is>
       </c>
       <c r="E29" s="8" t="n"/>
-      <c r="F29" s="44" t="inlineStr">
+      <c r="F29" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BE_BOUND.NON_MEM_SCHEDULER / SLOTS</t>
         </is>
       </c>
-      <c r="G29" s="44" t="n"/>
-      <c r="H29" s="44" t="n"/>
-      <c r="I29" s="44" t="inlineStr">
+      <c r="G29" s="7" t="n"/>
+      <c r="H29" s="7" t="n"/>
+      <c r="I29" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2363,22 +2395,22 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B30" s="59" t="n"/>
-      <c r="C30" s="59" t="n"/>
-      <c r="D30" s="71" t="inlineStr">
+      <c r="B30" s="63" t="n"/>
+      <c r="C30" s="63" t="n"/>
+      <c r="D30" s="74" t="inlineStr">
         <is>
           <t>Register</t>
         </is>
       </c>
       <c r="E30" s="8" t="n"/>
-      <c r="F30" s="44" t="inlineStr">
+      <c r="F30" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BE_BOUND.REGISTER / SLOTS</t>
         </is>
       </c>
-      <c r="G30" s="44" t="n"/>
-      <c r="H30" s="44" t="n"/>
-      <c r="I30" s="44" t="inlineStr">
+      <c r="G30" s="7" t="n"/>
+      <c r="H30" s="7" t="n"/>
+      <c r="I30" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2401,22 +2433,22 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B31" s="59" t="n"/>
-      <c r="C31" s="59" t="n"/>
-      <c r="D31" s="71" t="inlineStr">
+      <c r="B31" s="63" t="n"/>
+      <c r="C31" s="63" t="n"/>
+      <c r="D31" s="74" t="inlineStr">
         <is>
           <t>Reorder_Buffer</t>
         </is>
       </c>
       <c r="E31" s="8" t="n"/>
-      <c r="F31" s="44" t="inlineStr">
+      <c r="F31" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BE_BOUND.REORDER_BUFFER / SLOTS</t>
         </is>
       </c>
-      <c r="G31" s="44" t="n"/>
-      <c r="H31" s="44" t="n"/>
-      <c r="I31" s="44" t="inlineStr">
+      <c r="G31" s="7" t="n"/>
+      <c r="H31" s="7" t="n"/>
+      <c r="I31" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2439,22 +2471,22 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B32" s="59" t="n"/>
-      <c r="C32" s="59" t="n"/>
-      <c r="D32" s="71" t="inlineStr">
+      <c r="B32" s="63" t="n"/>
+      <c r="C32" s="63" t="n"/>
+      <c r="D32" s="74" t="inlineStr">
         <is>
           <t>Store_Buffer</t>
         </is>
       </c>
       <c r="E32" s="8" t="n"/>
-      <c r="F32" s="44" t="inlineStr">
+      <c r="F32" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BE_BOUND.STORE_BUFFER / SLOTS</t>
         </is>
       </c>
-      <c r="G32" s="44" t="n"/>
-      <c r="H32" s="44" t="n"/>
-      <c r="I32" s="44" t="inlineStr">
+      <c r="G32" s="7" t="n"/>
+      <c r="H32" s="7" t="n"/>
+      <c r="I32" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2477,22 +2509,22 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B33" s="59" t="n"/>
-      <c r="C33" s="59" t="n"/>
-      <c r="D33" s="71" t="inlineStr">
+      <c r="B33" s="63" t="n"/>
+      <c r="C33" s="63" t="n"/>
+      <c r="D33" s="74" t="inlineStr">
         <is>
           <t>Alloc_Restriction</t>
         </is>
       </c>
       <c r="E33" s="8" t="n"/>
-      <c r="F33" s="44" t="inlineStr">
+      <c r="F33" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BE_BOUND.ALLOC_RESTRICTIONS / SLOTS</t>
         </is>
       </c>
-      <c r="G33" s="44" t="n"/>
-      <c r="H33" s="44" t="n"/>
-      <c r="I33" s="44" t="inlineStr">
+      <c r="G33" s="7" t="n"/>
+      <c r="H33" s="7" t="n"/>
+      <c r="I33" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2515,22 +2547,22 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B34" s="59" t="n"/>
-      <c r="C34" s="59" t="n"/>
-      <c r="D34" s="71" t="inlineStr">
+      <c r="B34" s="63" t="n"/>
+      <c r="C34" s="63" t="n"/>
+      <c r="D34" s="74" t="inlineStr">
         <is>
           <t>Serialization</t>
         </is>
       </c>
       <c r="E34" s="8" t="n"/>
-      <c r="F34" s="44" t="inlineStr">
+      <c r="F34" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_BE_BOUND.SERIALIZATION / SLOTS</t>
         </is>
       </c>
-      <c r="G34" s="44" t="n"/>
-      <c r="H34" s="44" t="n"/>
-      <c r="I34" s="44" t="inlineStr">
+      <c r="G34" s="7" t="n"/>
+      <c r="H34" s="7" t="n"/>
+      <c r="I34" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2553,26 +2585,26 @@
           <t>RET</t>
         </is>
       </c>
-      <c r="B35" s="72" t="inlineStr">
+      <c r="B35" s="75" t="inlineStr">
         <is>
           <t>Retiring</t>
         </is>
       </c>
-      <c r="C35" s="64" t="n"/>
-      <c r="D35" s="64" t="n"/>
+      <c r="C35" s="57" t="n"/>
+      <c r="D35" s="57" t="n"/>
       <c r="E35" s="8" t="n"/>
-      <c r="F35" s="44" t="inlineStr">
+      <c r="F35" s="7" t="inlineStr">
         <is>
           <t>TOPDOWN_RETIRING.ALL / SLOTS</t>
         </is>
       </c>
-      <c r="G35" s="44" t="inlineStr">
+      <c r="G35" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">UOPS_RETIRED.ANY / SLOTS </t>
         </is>
       </c>
-      <c r="H35" s="44" t="n"/>
-      <c r="I35" s="44" t="inlineStr">
+      <c r="H35" s="7" t="n"/>
+      <c r="I35" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2595,22 +2627,22 @@
           <t>RET</t>
         </is>
       </c>
-      <c r="B36" s="59" t="n"/>
-      <c r="C36" s="73" t="inlineStr">
+      <c r="B36" s="63" t="n"/>
+      <c r="C36" s="76" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="D36" s="64" t="n"/>
+      <c r="D36" s="57" t="n"/>
       <c r="E36" s="8" t="n"/>
-      <c r="F36" s="44" t="inlineStr">
+      <c r="F36" s="7" t="inlineStr">
         <is>
           <t>( TOPDOWN_RETIRING.ALL - UOPS_RETIRED.MS ) / SLOTS</t>
         </is>
       </c>
-      <c r="G36" s="44" t="n"/>
-      <c r="H36" s="44" t="n"/>
-      <c r="I36" s="44" t="inlineStr">
+      <c r="G36" s="7" t="n"/>
+      <c r="H36" s="7" t="n"/>
+      <c r="I36" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2633,33 +2665,33 @@
           <t>RET</t>
         </is>
       </c>
-      <c r="B37" s="59" t="n"/>
-      <c r="C37" s="64" t="n"/>
-      <c r="D37" s="74" t="inlineStr">
-        <is>
-          <t>FP_uops</t>
+      <c r="B37" s="63" t="n"/>
+      <c r="C37" s="57" t="n"/>
+      <c r="D37" s="77" t="inlineStr">
+        <is>
+          <t>FPDIV_uops</t>
         </is>
       </c>
       <c r="E37" s="8" t="n"/>
-      <c r="F37" s="44" t="inlineStr">
+      <c r="F37" s="7" t="inlineStr">
         <is>
           <t>UOPS_RETIRED.FPDIV / SLOTS</t>
         </is>
       </c>
-      <c r="G37" s="44" t="inlineStr">
+      <c r="G37" s="7" t="inlineStr">
         <is>
           <t>UOPS_RETIRED.FPDIV / SLOTS</t>
         </is>
       </c>
-      <c r="H37" s="44" t="n"/>
-      <c r="I37" s="44" t="inlineStr">
+      <c r="H37" s="7" t="n"/>
+      <c r="I37" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
       </c>
       <c r="J37" s="8" t="inlineStr">
         <is>
-          <t>Counts the number of floating point operations per uop with all default weighting.</t>
+          <t>Counts the number of floating point divide operations per uop.</t>
         </is>
       </c>
       <c r="K37" s="8" t="n"/>
@@ -2675,22 +2707,22 @@
           <t>RET</t>
         </is>
       </c>
-      <c r="B38" s="59" t="n"/>
-      <c r="C38" s="64" t="n"/>
-      <c r="D38" s="74" t="inlineStr">
+      <c r="B38" s="63" t="n"/>
+      <c r="C38" s="57" t="n"/>
+      <c r="D38" s="77" t="inlineStr">
         <is>
           <t>Other_Ret</t>
         </is>
       </c>
       <c r="E38" s="8" t="n"/>
-      <c r="F38" s="44" t="inlineStr">
+      <c r="F38" s="7" t="inlineStr">
         <is>
           <t>( TOPDOWN_RETIRING.ALL - UOPS_RETIRED.MS - UOPS_RETIRED.FPDIV ) / SLOTS</t>
         </is>
       </c>
-      <c r="G38" s="44" t="n"/>
-      <c r="H38" s="44" t="n"/>
-      <c r="I38" s="44" t="inlineStr">
+      <c r="G38" s="7" t="n"/>
+      <c r="H38" s="7" t="n"/>
+      <c r="I38" s="7" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
@@ -2708,42 +2740,42 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="75" t="inlineStr">
+      <c r="A39" s="78" t="inlineStr">
         <is>
           <t>RET</t>
         </is>
       </c>
-      <c r="B39" s="75" t="n"/>
-      <c r="C39" s="76" t="inlineStr">
+      <c r="B39" s="78" t="n"/>
+      <c r="C39" s="79" t="inlineStr">
         <is>
           <t>MS_uops</t>
         </is>
       </c>
-      <c r="D39" s="75" t="n"/>
-      <c r="E39" s="75" t="n"/>
-      <c r="F39" s="77" t="inlineStr">
+      <c r="D39" s="78" t="n"/>
+      <c r="E39" s="78" t="n"/>
+      <c r="F39" s="80" t="inlineStr">
         <is>
           <t>UOPS_RETIRED.MS / SLOTS</t>
         </is>
       </c>
-      <c r="G39" s="77" t="inlineStr">
+      <c r="G39" s="80" t="inlineStr">
         <is>
           <t>UOPS_RETIRED.MS / SLOTS</t>
         </is>
       </c>
-      <c r="H39" s="77" t="n"/>
-      <c r="I39" s="77" t="inlineStr">
+      <c r="H39" s="80" t="n"/>
+      <c r="I39" s="80" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
       </c>
-      <c r="J39" s="75" t="inlineStr">
+      <c r="J39" s="78" t="inlineStr">
         <is>
           <t>Counts the number of uops that are from the complex flows issued by the micro-sequencer (MS).  This includes uops from flows due to complex instructions, faults, assists, and inserted flows.</t>
         </is>
       </c>
       <c r="K39" s="19" t="n"/>
-      <c r="L39" s="75" t="inlineStr">
+      <c r="L39" s="78" t="inlineStr">
         <is>
           <t>&gt;0.05</t>
         </is>
@@ -2763,10 +2795,10 @@
       <c r="C40" s="8" t="n"/>
       <c r="D40" s="8" t="n"/>
       <c r="E40" s="8" t="n"/>
-      <c r="F40" s="44" t="n"/>
-      <c r="G40" s="44" t="n"/>
-      <c r="H40" s="44" t="n"/>
-      <c r="I40" s="44" t="n"/>
+      <c r="F40" s="7" t="n"/>
+      <c r="G40" s="7" t="n"/>
+      <c r="H40" s="7" t="n"/>
+      <c r="I40" s="7" t="n"/>
       <c r="J40" s="8" t="n"/>
       <c r="K40" s="8" t="inlineStr">
         <is>
@@ -2789,18 +2821,18 @@
       <c r="C41" s="8" t="n"/>
       <c r="D41" s="8" t="n"/>
       <c r="E41" s="8" t="n"/>
-      <c r="F41" s="44" t="inlineStr">
+      <c r="F41" s="7" t="inlineStr">
         <is>
           <t>CPU_CLK_UNHALTED.CORE</t>
         </is>
       </c>
-      <c r="G41" s="44" t="inlineStr">
+      <c r="G41" s="7" t="inlineStr">
         <is>
           <t>CPU_CLK_UNHALTED.CORE</t>
         </is>
       </c>
-      <c r="H41" s="44" t="n"/>
-      <c r="I41" s="44" t="inlineStr">
+      <c r="H41" s="7" t="n"/>
+      <c r="I41" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2827,18 +2859,18 @@
       <c r="C42" s="8" t="n"/>
       <c r="D42" s="8" t="n"/>
       <c r="E42" s="8" t="n"/>
-      <c r="F42" s="44" t="inlineStr">
+      <c r="F42" s="7" t="inlineStr">
         <is>
           <t>CPU_CLK_UNHALTED.CORE_P</t>
         </is>
       </c>
-      <c r="G42" s="44" t="inlineStr">
+      <c r="G42" s="7" t="inlineStr">
         <is>
           <t>CPU_CLK_UNHALTED.CORE_P</t>
         </is>
       </c>
-      <c r="H42" s="44" t="n"/>
-      <c r="I42" s="44" t="inlineStr">
+      <c r="H42" s="7" t="n"/>
+      <c r="I42" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2865,18 +2897,18 @@
       <c r="C43" s="8" t="n"/>
       <c r="D43" s="8" t="n"/>
       <c r="E43" s="8" t="n"/>
-      <c r="F43" s="44" t="inlineStr">
+      <c r="F43" s="7" t="inlineStr">
         <is>
           <t>#Pipeline_Width * CLKS</t>
         </is>
       </c>
-      <c r="G43" s="44" t="inlineStr">
+      <c r="G43" s="7" t="inlineStr">
         <is>
           <t>#Pipeline_Width * CLKS</t>
         </is>
       </c>
-      <c r="H43" s="44" t="n"/>
-      <c r="I43" s="44" t="inlineStr">
+      <c r="H43" s="7" t="n"/>
+      <c r="I43" s="7" t="inlineStr">
         <is>
           <t>Cycles</t>
         </is>
@@ -2903,18 +2935,18 @@
       <c r="C44" s="8" t="n"/>
       <c r="D44" s="8" t="n"/>
       <c r="E44" s="8" t="n"/>
-      <c r="F44" s="44" t="inlineStr">
+      <c r="F44" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / CLKS</t>
         </is>
       </c>
-      <c r="G44" s="44" t="inlineStr">
+      <c r="G44" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / CLKS</t>
         </is>
       </c>
-      <c r="H44" s="44" t="n"/>
-      <c r="I44" s="44" t="n"/>
+      <c r="H44" s="7" t="n"/>
+      <c r="I44" s="7" t="n"/>
       <c r="J44" s="8" t="inlineStr">
         <is>
           <t>Instructions Per Cycle</t>
@@ -2941,18 +2973,18 @@
       <c r="C45" s="8" t="n"/>
       <c r="D45" s="8" t="n"/>
       <c r="E45" s="8" t="n"/>
-      <c r="F45" s="44" t="inlineStr">
+      <c r="F45" s="7" t="inlineStr">
         <is>
           <t>CLKS / INST_RETIRED.ANY</t>
         </is>
       </c>
-      <c r="G45" s="44" t="inlineStr">
+      <c r="G45" s="7" t="inlineStr">
         <is>
           <t>CLKS / INST_RETIRED.ANY</t>
         </is>
       </c>
-      <c r="H45" s="44" t="n"/>
-      <c r="I45" s="44" t="n"/>
+      <c r="H45" s="7" t="n"/>
+      <c r="I45" s="7" t="n"/>
       <c r="J45" s="8" t="inlineStr">
         <is>
           <t>Cycles Per Instruction</t>
@@ -2979,18 +3011,18 @@
       <c r="C46" s="8" t="n"/>
       <c r="D46" s="8" t="n"/>
       <c r="E46" s="8" t="n"/>
-      <c r="F46" s="44" t="inlineStr">
+      <c r="F46" s="7" t="inlineStr">
         <is>
           <t>UOPS_RETIRED.ALL / INST_RETIRED.ANY</t>
         </is>
       </c>
-      <c r="G46" s="44" t="inlineStr">
+      <c r="G46" s="7" t="inlineStr">
         <is>
           <t>UOPS_RETIRED.ANY / INST_RETIRED.ANY</t>
         </is>
       </c>
-      <c r="H46" s="44" t="n"/>
-      <c r="I46" s="44" t="n"/>
+      <c r="H46" s="7" t="n"/>
+      <c r="I46" s="7" t="n"/>
       <c r="J46" s="8" t="inlineStr">
         <is>
           <t>Uops Per Instruction</t>
@@ -3017,18 +3049,18 @@
       <c r="C47" s="8" t="n"/>
       <c r="D47" s="8" t="n"/>
       <c r="E47" s="8" t="n"/>
-      <c r="F47" s="44" t="inlineStr">
+      <c r="F47" s="7" t="inlineStr">
         <is>
           <t>100 * LD_BLOCKS.DATA_UNKNOWN / MEM_UOPS_RETIRED.ALL_LOADS</t>
         </is>
       </c>
-      <c r="G47" s="44" t="inlineStr">
+      <c r="G47" s="7" t="inlineStr">
         <is>
           <t>100 * LD_BLOCKS.DATA_UNKNOWN / MEM_UOPS_RETIRED.ALL_LOADS</t>
         </is>
       </c>
-      <c r="H47" s="44" t="n"/>
-      <c r="I47" s="44" t="n"/>
+      <c r="H47" s="7" t="n"/>
+      <c r="I47" s="7" t="n"/>
       <c r="J47" s="8" t="inlineStr">
         <is>
           <t>Percentage of total non-speculative loads with a store forward or unknown store address block</t>
@@ -3051,18 +3083,18 @@
       <c r="C48" s="8" t="n"/>
       <c r="D48" s="8" t="n"/>
       <c r="E48" s="8" t="n"/>
-      <c r="F48" s="44" t="inlineStr">
+      <c r="F48" s="7" t="inlineStr">
         <is>
           <t>100 * LD_BLOCKS.4K_ALIAS / MEM_UOPS_RETIRED.ALL_LOADS</t>
         </is>
       </c>
-      <c r="G48" s="44" t="inlineStr">
+      <c r="G48" s="7" t="inlineStr">
         <is>
           <t>100 * LD_BLOCKS.4K_ALIAS / MEM_UOPS_RETIRED.ALL_LOADS</t>
         </is>
       </c>
-      <c r="H48" s="44" t="n"/>
-      <c r="I48" s="44" t="n"/>
+      <c r="H48" s="7" t="n"/>
+      <c r="I48" s="7" t="n"/>
       <c r="J48" s="8" t="inlineStr">
         <is>
           <t>Percentage of total non-speculative loads with a address aliasing block</t>
@@ -3085,18 +3117,18 @@
       <c r="C49" s="8" t="n"/>
       <c r="D49" s="8" t="n"/>
       <c r="E49" s="8" t="n"/>
-      <c r="F49" s="44" t="inlineStr">
+      <c r="F49" s="7" t="inlineStr">
         <is>
           <t>100 * MEM_UOPS_RETIRED.SPLIT_LOADS / MEM_UOPS_RETIRED.ALL_LOADS</t>
         </is>
       </c>
-      <c r="G49" s="44" t="inlineStr">
+      <c r="G49" s="7" t="inlineStr">
         <is>
           <t>100 * MEM_UOPS_RETIRED.SPLIT_LOADS / MEM_UOPS_RETIRED.ALL_LOADS</t>
         </is>
       </c>
-      <c r="H49" s="44" t="n"/>
-      <c r="I49" s="44" t="n"/>
+      <c r="H49" s="7" t="n"/>
+      <c r="I49" s="7" t="n"/>
       <c r="J49" s="8" t="inlineStr">
         <is>
           <t>Percentage of total non-speculative loads that are splits</t>
@@ -3117,20 +3149,20 @@
         </is>
       </c>
       <c r="C50" s="8" t="n"/>
-      <c r="D50" s="64" t="n"/>
+      <c r="D50" s="57" t="n"/>
       <c r="E50" s="8" t="n"/>
-      <c r="F50" s="44" t="inlineStr">
+      <c r="F50" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / BR_INST_RETIRED.ALL_BRANCHES</t>
         </is>
       </c>
-      <c r="G50" s="44" t="inlineStr">
+      <c r="G50" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / BR_INST_RETIRED.ALL_BRANCHES</t>
         </is>
       </c>
-      <c r="H50" s="44" t="n"/>
-      <c r="I50" s="44" t="n"/>
+      <c r="H50" s="7" t="n"/>
+      <c r="I50" s="7" t="n"/>
       <c r="J50" s="8" t="inlineStr">
         <is>
           <t>Instructions per Branch (lower number means higher occurance rate)</t>
@@ -3157,18 +3189,18 @@
       <c r="C51" s="8" t="n"/>
       <c r="D51" s="8" t="n"/>
       <c r="E51" s="8" t="n"/>
-      <c r="F51" s="44" t="inlineStr">
+      <c r="F51" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / BR_INST_RETIRED.CALL</t>
         </is>
       </c>
-      <c r="G51" s="44" t="inlineStr">
+      <c r="G51" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / BR_INST_RETIRED.CALL</t>
         </is>
       </c>
-      <c r="H51" s="44" t="n"/>
-      <c r="I51" s="44" t="n"/>
+      <c r="H51" s="7" t="n"/>
+      <c r="I51" s="7" t="n"/>
       <c r="J51" s="8" t="inlineStr">
         <is>
           <t>Instruction per (near) call (lower number means higher occurance rate)</t>
@@ -3195,18 +3227,18 @@
       <c r="C52" s="8" t="n"/>
       <c r="D52" s="8" t="n"/>
       <c r="E52" s="8" t="n"/>
-      <c r="F52" s="44" t="inlineStr">
+      <c r="F52" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / MEM_UOPS_RETIRED.ALL_LOADS</t>
         </is>
       </c>
-      <c r="G52" s="44" t="inlineStr">
+      <c r="G52" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / MEM_UOPS_RETIRED.ALL_LOADS</t>
         </is>
       </c>
-      <c r="H52" s="44" t="n"/>
-      <c r="I52" s="44" t="n"/>
+      <c r="H52" s="7" t="n"/>
+      <c r="I52" s="7" t="n"/>
       <c r="J52" s="8" t="inlineStr">
         <is>
           <t>Instructions per Load</t>
@@ -3233,18 +3265,18 @@
       <c r="C53" s="8" t="n"/>
       <c r="D53" s="8" t="n"/>
       <c r="E53" s="8" t="n"/>
-      <c r="F53" s="44" t="inlineStr">
+      <c r="F53" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / MEM_UOPS_RETIRED.ALL_STORES</t>
         </is>
       </c>
-      <c r="G53" s="44" t="inlineStr">
+      <c r="G53" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / MEM_UOPS_RETIRED.ALL_STORES</t>
         </is>
       </c>
-      <c r="H53" s="44" t="n"/>
-      <c r="I53" s="44" t="n"/>
+      <c r="H53" s="7" t="n"/>
+      <c r="I53" s="7" t="n"/>
       <c r="J53" s="8" t="inlineStr">
         <is>
           <t>Instructions per Store</t>
@@ -3271,21 +3303,21 @@
       <c r="C54" s="8" t="n"/>
       <c r="D54" s="8" t="n"/>
       <c r="E54" s="8" t="n"/>
-      <c r="F54" s="44" t="inlineStr">
+      <c r="F54" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / BR_MISP_RETIRED.ALL_BRANCHES</t>
         </is>
       </c>
-      <c r="G54" s="44" t="inlineStr">
+      <c r="G54" s="7" t="inlineStr">
         <is>
           <t>INST_RETIRED.ANY / BR_MISP_RETIRED.ALL_BRANCHES</t>
         </is>
       </c>
-      <c r="H54" s="44" t="n"/>
-      <c r="I54" s="44" t="n"/>
+      <c r="H54" s="7" t="n"/>
+      <c r="I54" s="7" t="n"/>
       <c r="J54" s="8" t="inlineStr">
         <is>
-          <t>Number of Instructions per non-speculative Branch Misprediction</t>
+          <t>Instructions per retired Branch Misprediction</t>
         </is>
       </c>
       <c r="K54" s="8" t="inlineStr">
@@ -3296,155 +3328,139 @@
       <c r="L54" s="8" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="8" t="inlineStr">
+      <c r="A55" s="57" t="inlineStr">
         <is>
           <t>Info.Inst_Mix</t>
         </is>
       </c>
-      <c r="B55" s="8" t="inlineStr">
-        <is>
-          <t>IpFarBranch</t>
-        </is>
-      </c>
-      <c r="C55" s="8" t="n"/>
-      <c r="D55" s="8" t="n"/>
-      <c r="E55" s="8" t="n"/>
-      <c r="F55" s="44" t="inlineStr">
-        <is>
-          <t>INST_RETIRED.ANY / ( BR_INST_RETIRED.FAR_BRANCH / 2 )</t>
-        </is>
-      </c>
-      <c r="G55" s="44" t="inlineStr">
-        <is>
-          <t xml:space="preserve">INST_RETIRED.ANY / ( BR_INST_RETIRED.FAR_BRANCH / 2 ) </t>
-        </is>
-      </c>
-      <c r="H55" s="44" t="n"/>
-      <c r="I55" s="44" t="n"/>
-      <c r="J55" s="8" t="inlineStr">
-        <is>
-          <t>Instructions per Far Branch</t>
-        </is>
-      </c>
-      <c r="K55" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="B55" s="57" t="inlineStr">
+        <is>
+          <t>IpMisp_Cond_Ntaken</t>
+        </is>
+      </c>
+      <c r="C55" s="57" t="n"/>
+      <c r="D55" s="57" t="n"/>
+      <c r="E55" s="57" t="n"/>
+      <c r="F55" s="41" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / ( BR_MISP_RETIRED.JCC - BR_MISP_RETIRED.TAKEN_JCC)</t>
+        </is>
+      </c>
+      <c r="G55" s="41" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / ( BR_MISP_RETIRED.JCC - BR_MISP_RETIRED.TAKEN_JCC)</t>
+        </is>
+      </c>
+      <c r="H55" s="41" t="n"/>
+      <c r="I55" s="41" t="n"/>
+      <c r="J55" s="57" t="inlineStr">
+        <is>
+          <t>Instructions per retired conditional Branch Misprediction where the branch was not taken</t>
+        </is>
+      </c>
+      <c r="K55" s="8" t="n"/>
       <c r="L55" s="8" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="8" t="inlineStr">
+      <c r="A56" s="57" t="inlineStr">
         <is>
           <t>Info.Inst_Mix</t>
         </is>
       </c>
-      <c r="B56" s="8" t="inlineStr">
-        <is>
-          <t>Branch_Mispredict_Ratio</t>
-        </is>
-      </c>
-      <c r="C56" s="8" t="n"/>
-      <c r="D56" s="8" t="n"/>
-      <c r="E56" s="8" t="n"/>
-      <c r="F56" s="44" t="inlineStr">
-        <is>
-          <t>BR_MISP_RETIRED.ALL_BRANCHES / BR_INST_RETIRED.ALL_BRANCHES</t>
-        </is>
-      </c>
-      <c r="G56" s="44" t="inlineStr">
-        <is>
-          <t>BR_MISP_RETIRED.ALL_BRANCHES / BR_INST_RETIRED.ALL_BRANCHES</t>
-        </is>
-      </c>
-      <c r="H56" s="44" t="n"/>
-      <c r="I56" s="44" t="n"/>
-      <c r="J56" s="8" t="inlineStr">
-        <is>
-          <t>Ratio of all branches which mispredict</t>
-        </is>
-      </c>
-      <c r="K56" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="B56" s="57" t="inlineStr">
+        <is>
+          <t>IpMisp_Cond_Taken</t>
+        </is>
+      </c>
+      <c r="C56" s="57" t="n"/>
+      <c r="D56" s="57" t="n"/>
+      <c r="E56" s="57" t="n"/>
+      <c r="F56" s="41" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / BR_MISP_RETIRED.TAKEN_JCC</t>
+        </is>
+      </c>
+      <c r="G56" s="41" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / BR_MISP_RETIRED.TAKEN_JCC</t>
+        </is>
+      </c>
+      <c r="H56" s="41" t="n"/>
+      <c r="I56" s="41" t="n"/>
+      <c r="J56" s="57" t="inlineStr">
+        <is>
+          <t>Instructions per retired conditional Branch Misprediction where the branch was taken</t>
+        </is>
+      </c>
+      <c r="K56" s="8" t="n"/>
       <c r="L56" s="8" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="8" t="inlineStr">
+      <c r="A57" s="57" t="inlineStr">
         <is>
           <t>Info.Inst_Mix</t>
         </is>
       </c>
-      <c r="B57" s="8" t="inlineStr">
-        <is>
-          <t>Branch_Mispredict_to_Unknown_Branch_Ratio</t>
-        </is>
-      </c>
-      <c r="C57" s="8" t="n"/>
-      <c r="D57" s="8" t="n"/>
-      <c r="E57" s="8" t="n"/>
-      <c r="F57" s="44" t="inlineStr">
-        <is>
-          <t>BR_MISP_RETIRED.ALL_BRANCHES / BACLEARS.ANY</t>
-        </is>
-      </c>
-      <c r="G57" s="44" t="inlineStr">
-        <is>
-          <t>BR_MISP_RETIRED.ALL_BRANCHES / BACLEARS.ALL</t>
-        </is>
-      </c>
-      <c r="H57" s="44" t="n"/>
-      <c r="I57" s="44" t="n"/>
-      <c r="J57" s="8" t="inlineStr">
-        <is>
-          <t>Ratio between Mispredicted branches and unknown branches</t>
-        </is>
-      </c>
-      <c r="K57" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="B57" s="57" t="inlineStr">
+        <is>
+          <t>IpMisp_Ret</t>
+        </is>
+      </c>
+      <c r="C57" s="57" t="n"/>
+      <c r="D57" s="57" t="n"/>
+      <c r="E57" s="57" t="n"/>
+      <c r="F57" s="41" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / BR_MISP_RETIRED.RETURN</t>
+        </is>
+      </c>
+      <c r="G57" s="41" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / BR_MISP_RETIRED.RETURN</t>
+        </is>
+      </c>
+      <c r="H57" s="41" t="n"/>
+      <c r="I57" s="41" t="n"/>
+      <c r="J57" s="57" t="inlineStr">
+        <is>
+          <t>Instructions per retired return Branch Misprediction</t>
+        </is>
+      </c>
+      <c r="K57" s="8" t="n"/>
       <c r="L57" s="8" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="8" t="inlineStr">
+      <c r="A58" s="57" t="inlineStr">
         <is>
           <t>Info.Inst_Mix</t>
         </is>
       </c>
-      <c r="B58" s="8" t="inlineStr">
-        <is>
-          <t>Microcode_Uop_Ratio</t>
-        </is>
-      </c>
-      <c r="C58" s="8" t="n"/>
-      <c r="D58" s="8" t="n"/>
-      <c r="E58" s="8" t="n"/>
-      <c r="F58" s="44" t="inlineStr">
-        <is>
-          <t>100 * UOPS_RETIRED.MS / UOPS_RETIRED.ALL</t>
-        </is>
-      </c>
-      <c r="G58" s="44" t="inlineStr">
-        <is>
-          <t>100 * UOPS_RETIRED.MS / UOPS_RETIRED.ANY</t>
-        </is>
-      </c>
-      <c r="H58" s="44" t="n"/>
-      <c r="I58" s="44" t="n"/>
-      <c r="J58" s="8" t="inlineStr">
-        <is>
-          <t>Percentage of all uops which are ucode ops</t>
-        </is>
-      </c>
-      <c r="K58" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="B58" s="57" t="inlineStr">
+        <is>
+          <t>IpMisp_Indirect</t>
+        </is>
+      </c>
+      <c r="C58" s="57" t="n"/>
+      <c r="D58" s="57" t="n"/>
+      <c r="E58" s="57" t="n"/>
+      <c r="F58" s="41" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / BR_MISP_RETIRED.NON_RETURN_IND</t>
+        </is>
+      </c>
+      <c r="G58" s="41" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / BR_MISP_RETIRED.NON_RETURN_IND</t>
+        </is>
+      </c>
+      <c r="H58" s="41" t="n"/>
+      <c r="I58" s="41" t="n"/>
+      <c r="J58" s="57" t="inlineStr">
+        <is>
+          <t>Instructions per retired indirect call or jump Branch Misprediction</t>
+        </is>
+      </c>
+      <c r="K58" s="8" t="n"/>
       <c r="L58" s="8" t="n"/>
     </row>
     <row r="59">
@@ -3455,27 +3471,27 @@
       </c>
       <c r="B59" s="8" t="inlineStr">
         <is>
-          <t>FPDiv_Uop_Ratio</t>
+          <t>IpFarBranch</t>
         </is>
       </c>
       <c r="C59" s="8" t="n"/>
       <c r="D59" s="8" t="n"/>
       <c r="E59" s="8" t="n"/>
-      <c r="F59" s="44" t="inlineStr">
-        <is>
-          <t>100 * UOPS_RETIRED.FPDIV / UOPS_RETIRED.ALL</t>
-        </is>
-      </c>
-      <c r="G59" s="44" t="inlineStr">
-        <is>
-          <t>100 * UOPS_RETIRED.FPDIV / UOPS_RETIRED.ANY</t>
-        </is>
-      </c>
-      <c r="H59" s="44" t="n"/>
-      <c r="I59" s="44" t="n"/>
+      <c r="F59" s="7" t="inlineStr">
+        <is>
+          <t>INST_RETIRED.ANY / ( BR_INST_RETIRED.FAR_BRANCH / 2 )</t>
+        </is>
+      </c>
+      <c r="G59" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INST_RETIRED.ANY / ( BR_INST_RETIRED.FAR_BRANCH / 2 ) </t>
+        </is>
+      </c>
+      <c r="H59" s="7" t="n"/>
+      <c r="I59" s="7" t="n"/>
       <c r="J59" s="8" t="inlineStr">
         <is>
-          <t>Percentage of all uops which are FPDiv uops</t>
+          <t>Instructions per Far Branch</t>
         </is>
       </c>
       <c r="K59" s="8" t="inlineStr">
@@ -3493,27 +3509,27 @@
       </c>
       <c r="B60" s="8" t="inlineStr">
         <is>
-          <t>IDiv_Uop_Ratio</t>
+          <t>Branch_Mispredict_Ratio</t>
         </is>
       </c>
       <c r="C60" s="8" t="n"/>
       <c r="D60" s="8" t="n"/>
       <c r="E60" s="8" t="n"/>
-      <c r="F60" s="44" t="inlineStr">
-        <is>
-          <t>100 * UOPS_RETIRED.IDIV / UOPS_RETIRED.ALL</t>
-        </is>
-      </c>
-      <c r="G60" s="44" t="inlineStr">
-        <is>
-          <t>100 * UOPS_RETIRED.IDIV / UOPS_RETIRED.ANY</t>
-        </is>
-      </c>
-      <c r="H60" s="44" t="n"/>
-      <c r="I60" s="44" t="n"/>
+      <c r="F60" s="7" t="inlineStr">
+        <is>
+          <t>BR_MISP_RETIRED.ALL_BRANCHES / BR_INST_RETIRED.ALL_BRANCHES</t>
+        </is>
+      </c>
+      <c r="G60" s="7" t="inlineStr">
+        <is>
+          <t>BR_MISP_RETIRED.ALL_BRANCHES / BR_INST_RETIRED.ALL_BRANCHES</t>
+        </is>
+      </c>
+      <c r="H60" s="7" t="n"/>
+      <c r="I60" s="7" t="n"/>
       <c r="J60" s="8" t="inlineStr">
         <is>
-          <t>Percentage of all uops which are IDiv uops</t>
+          <t>Ratio of all branches which mispredict</t>
         </is>
       </c>
       <c r="K60" s="8" t="inlineStr">
@@ -3531,23 +3547,27 @@
       </c>
       <c r="B61" s="8" t="inlineStr">
         <is>
-          <t>X87_Uop_Ratio</t>
+          <t>Branch_Mispredict_to_Unknown_Branch_Ratio</t>
         </is>
       </c>
       <c r="C61" s="8" t="n"/>
       <c r="D61" s="8" t="n"/>
       <c r="E61" s="8" t="n"/>
-      <c r="F61" s="44" t="inlineStr">
-        <is>
-          <t>100 * UOPS_RETIRED.X87 / UOPS_RETIRED.ALL</t>
-        </is>
-      </c>
-      <c r="G61" s="44" t="n"/>
-      <c r="H61" s="44" t="n"/>
-      <c r="I61" s="44" t="n"/>
+      <c r="F61" s="7" t="inlineStr">
+        <is>
+          <t>BR_MISP_RETIRED.ALL_BRANCHES / BACLEARS.ANY</t>
+        </is>
+      </c>
+      <c r="G61" s="7" t="inlineStr">
+        <is>
+          <t>BR_MISP_RETIRED.ALL_BRANCHES / BACLEARS.ALL</t>
+        </is>
+      </c>
+      <c r="H61" s="7" t="n"/>
+      <c r="I61" s="7" t="n"/>
       <c r="J61" s="8" t="inlineStr">
         <is>
-          <t>Percentage of all uops which are x87 uops</t>
+          <t>Ratio between Mispredicted branches and unknown branches</t>
         </is>
       </c>
       <c r="K61" s="8" t="inlineStr">
@@ -3560,32 +3580,32 @@
     <row r="62">
       <c r="A62" s="8" t="inlineStr">
         <is>
-          <t>Info.System</t>
+          <t>Info.Inst_Mix</t>
         </is>
       </c>
       <c r="B62" s="8" t="inlineStr">
         <is>
-          <t>Turbo_Utilization</t>
+          <t>Microcode_Uop_Ratio</t>
         </is>
       </c>
       <c r="C62" s="8" t="n"/>
       <c r="D62" s="8" t="n"/>
       <c r="E62" s="8" t="n"/>
-      <c r="F62" s="44" t="inlineStr">
-        <is>
-          <t>CLKS / CPU_CLK_UNHALTED.REF_TSC</t>
-        </is>
-      </c>
-      <c r="G62" s="44" t="inlineStr">
-        <is>
-          <t>CLKS / CPU_CLK_UNHALTED.REF_TSC</t>
-        </is>
-      </c>
-      <c r="H62" s="44" t="n"/>
-      <c r="I62" s="44" t="n"/>
+      <c r="F62" s="7" t="inlineStr">
+        <is>
+          <t>100 * UOPS_RETIRED.MS / UOPS_RETIRED.ALL</t>
+        </is>
+      </c>
+      <c r="G62" s="7" t="inlineStr">
+        <is>
+          <t>100 * UOPS_RETIRED.MS / UOPS_RETIRED.ANY</t>
+        </is>
+      </c>
+      <c r="H62" s="7" t="n"/>
+      <c r="I62" s="7" t="n"/>
       <c r="J62" s="8" t="inlineStr">
         <is>
-          <t>Average Frequency Utilization relative nominal frequency</t>
+          <t>Percentage of all uops which are ucode ops</t>
         </is>
       </c>
       <c r="K62" s="8" t="inlineStr">
@@ -3598,32 +3618,32 @@
     <row r="63">
       <c r="A63" s="8" t="inlineStr">
         <is>
-          <t>Info.System</t>
+          <t>Info.Inst_Mix</t>
         </is>
       </c>
       <c r="B63" s="8" t="inlineStr">
         <is>
-          <t>Kernel_Utilization</t>
+          <t>FPDiv_Uop_Ratio</t>
         </is>
       </c>
       <c r="C63" s="8" t="n"/>
       <c r="D63" s="8" t="n"/>
       <c r="E63" s="8" t="n"/>
-      <c r="F63" s="44" t="inlineStr">
-        <is>
-          <t>CPU_CLK_UNHALTED.CORE_P:sup / CPU_CLK_UNHALTED.CORE_P</t>
-        </is>
-      </c>
-      <c r="G63" s="44" t="inlineStr">
-        <is>
-          <t>CPU_CLK_UNHALTED.CORE_P:sup / CPU_CLK_UNHALTED.CORE_P</t>
-        </is>
-      </c>
-      <c r="H63" s="44" t="n"/>
-      <c r="I63" s="44" t="n"/>
+      <c r="F63" s="7" t="inlineStr">
+        <is>
+          <t>100 * UOPS_RETIRED.FPDIV / UOPS_RETIRED.ALL</t>
+        </is>
+      </c>
+      <c r="G63" s="7" t="inlineStr">
+        <is>
+          <t>100 * UOPS_RETIRED.FPDIV / UOPS_RETIRED.ANY</t>
+        </is>
+      </c>
+      <c r="H63" s="7" t="n"/>
+      <c r="I63" s="7" t="n"/>
       <c r="J63" s="8" t="inlineStr">
         <is>
-          <t>Fraction of cycles spent in Kernel mode</t>
+          <t>Percentage of all uops which are FPDiv uops</t>
         </is>
       </c>
       <c r="K63" s="8" t="inlineStr">
@@ -3636,32 +3656,32 @@
     <row r="64">
       <c r="A64" s="8" t="inlineStr">
         <is>
-          <t>Info.System</t>
+          <t>Info.Inst_Mix</t>
         </is>
       </c>
       <c r="B64" s="8" t="inlineStr">
         <is>
-          <t>CPU_Utilization</t>
+          <t>IDiv_Uop_Ratio</t>
         </is>
       </c>
       <c r="C64" s="8" t="n"/>
       <c r="D64" s="8" t="n"/>
       <c r="E64" s="8" t="n"/>
-      <c r="F64" s="44" t="inlineStr">
-        <is>
-          <t>CPU_CLK_UNHALTED.REF_TSC / TSC</t>
-        </is>
-      </c>
-      <c r="G64" s="44" t="inlineStr">
-        <is>
-          <t>CPU_CLK_UNHALTED.REF_TSC / TSC</t>
-        </is>
-      </c>
-      <c r="H64" s="44" t="n"/>
-      <c r="I64" s="44" t="n"/>
-      <c r="J64" s="78" t="inlineStr">
-        <is>
-          <t>Average CPU Utilization</t>
+      <c r="F64" s="7" t="inlineStr">
+        <is>
+          <t>100 * UOPS_RETIRED.IDIV / UOPS_RETIRED.ALL</t>
+        </is>
+      </c>
+      <c r="G64" s="7" t="inlineStr">
+        <is>
+          <t>100 * UOPS_RETIRED.IDIV / UOPS_RETIRED.ANY</t>
+        </is>
+      </c>
+      <c r="H64" s="7" t="n"/>
+      <c r="I64" s="7" t="n"/>
+      <c r="J64" s="8" t="inlineStr">
+        <is>
+          <t>Percentage of all uops which are IDiv uops</t>
         </is>
       </c>
       <c r="K64" s="8" t="inlineStr">
@@ -3674,28 +3694,28 @@
     <row r="65">
       <c r="A65" s="8" t="inlineStr">
         <is>
-          <t>Info.Memory</t>
+          <t>Info.Inst_Mix</t>
         </is>
       </c>
       <c r="B65" s="8" t="inlineStr">
         <is>
-          <t>Cycles_per_Demand_Load_L2_Hit</t>
+          <t>X87_Uop_Ratio</t>
         </is>
       </c>
       <c r="C65" s="8" t="n"/>
       <c r="D65" s="8" t="n"/>
       <c r="E65" s="8" t="n"/>
-      <c r="F65" s="44" t="inlineStr">
-        <is>
-          <t>MEM_BOUND_STALLS.LOAD_L2_HIT / MEM_LOAD_UOPS_RETIRED.L2_HIT</t>
-        </is>
-      </c>
-      <c r="G65" s="44" t="n"/>
-      <c r="H65" s="44" t="n"/>
-      <c r="I65" s="44" t="n"/>
+      <c r="F65" s="7" t="inlineStr">
+        <is>
+          <t>100 * UOPS_RETIRED.X87 / UOPS_RETIRED.ALL</t>
+        </is>
+      </c>
+      <c r="G65" s="7" t="n"/>
+      <c r="H65" s="7" t="n"/>
+      <c r="I65" s="7" t="n"/>
       <c r="J65" s="8" t="inlineStr">
         <is>
-          <t>Cycle cost per L2 hit</t>
+          <t>Percentage of all uops which are x87 uops</t>
         </is>
       </c>
       <c r="K65" s="8" t="inlineStr">
@@ -3708,28 +3728,32 @@
     <row r="66">
       <c r="A66" s="8" t="inlineStr">
         <is>
-          <t>Info.Memory</t>
+          <t>Info.System</t>
         </is>
       </c>
       <c r="B66" s="8" t="inlineStr">
         <is>
-          <t>Cycles_per_Demand_Load_L3_Hit</t>
+          <t>Turbo_Utilization</t>
         </is>
       </c>
       <c r="C66" s="8" t="n"/>
       <c r="D66" s="8" t="n"/>
       <c r="E66" s="8" t="n"/>
-      <c r="F66" s="44" t="inlineStr">
-        <is>
-          <t>MEM_BOUND_STALLS.LOAD_LLC_HIT / MEM_LOAD_UOPS_RETIRED.L3_HIT</t>
-        </is>
-      </c>
-      <c r="G66" s="44" t="n"/>
-      <c r="H66" s="44" t="n"/>
-      <c r="I66" s="44" t="n"/>
+      <c r="F66" s="7" t="inlineStr">
+        <is>
+          <t>CLKS / CPU_CLK_UNHALTED.REF_TSC</t>
+        </is>
+      </c>
+      <c r="G66" s="7" t="inlineStr">
+        <is>
+          <t>CLKS / CPU_CLK_UNHALTED.REF_TSC</t>
+        </is>
+      </c>
+      <c r="H66" s="7" t="n"/>
+      <c r="I66" s="7" t="n"/>
       <c r="J66" s="8" t="inlineStr">
         <is>
-          <t>Cycle cost per LLC hit</t>
+          <t>Average Frequency Utilization relative nominal frequency</t>
         </is>
       </c>
       <c r="K66" s="8" t="inlineStr">
@@ -3742,28 +3766,32 @@
     <row r="67">
       <c r="A67" s="8" t="inlineStr">
         <is>
-          <t>Info.Memory</t>
+          <t>Info.System</t>
         </is>
       </c>
       <c r="B67" s="8" t="inlineStr">
         <is>
-          <t>Cycles_per_Demand_Load_DRAM_Hit</t>
+          <t>Kernel_Utilization</t>
         </is>
       </c>
       <c r="C67" s="8" t="n"/>
       <c r="D67" s="8" t="n"/>
       <c r="E67" s="8" t="n"/>
-      <c r="F67" s="44" t="inlineStr">
-        <is>
-          <t>MEM_BOUND_STALLS.LOAD_DRAM_HIT / MEM_LOAD_UOPS_RETIRED.DRAM_HIT</t>
-        </is>
-      </c>
-      <c r="G67" s="44" t="n"/>
-      <c r="H67" s="44" t="n"/>
-      <c r="I67" s="44" t="n"/>
+      <c r="F67" s="7" t="inlineStr">
+        <is>
+          <t>CPU_CLK_UNHALTED.CORE_P:sup / CPU_CLK_UNHALTED.CORE_P</t>
+        </is>
+      </c>
+      <c r="G67" s="7" t="inlineStr">
+        <is>
+          <t>CPU_CLK_UNHALTED.CORE_P:sup / CPU_CLK_UNHALTED.CORE_P</t>
+        </is>
+      </c>
+      <c r="H67" s="7" t="n"/>
+      <c r="I67" s="7" t="n"/>
       <c r="J67" s="8" t="inlineStr">
         <is>
-          <t>Cycle cost per DRAM hit</t>
+          <t>Fraction of cycles spent in Kernel mode</t>
         </is>
       </c>
       <c r="K67" s="8" t="inlineStr">
@@ -3776,28 +3804,32 @@
     <row r="68">
       <c r="A68" s="8" t="inlineStr">
         <is>
-          <t>Info.Frontend</t>
+          <t>Info.System</t>
         </is>
       </c>
       <c r="B68" s="8" t="inlineStr">
         <is>
-          <t>Inst_Miss_Cost_L2Hit_Percent</t>
+          <t>CPU_Utilization</t>
         </is>
       </c>
       <c r="C68" s="8" t="n"/>
       <c r="D68" s="8" t="n"/>
       <c r="E68" s="8" t="n"/>
-      <c r="F68" s="44" t="inlineStr">
-        <is>
-          <t>100 * MEM_BOUND_STALLS.IFETCH_L2_HIT / ( MEM_BOUND_STALLS.IFETCH )</t>
-        </is>
-      </c>
-      <c r="G68" s="44" t="n"/>
-      <c r="H68" s="44" t="n"/>
-      <c r="I68" s="44" t="n"/>
-      <c r="J68" s="8" t="inlineStr">
-        <is>
-          <t>Percent of instruction miss cost that hit in the L2</t>
+      <c r="F68" s="7" t="inlineStr">
+        <is>
+          <t>CPU_CLK_UNHALTED.REF_TSC / TSC</t>
+        </is>
+      </c>
+      <c r="G68" s="7" t="inlineStr">
+        <is>
+          <t>CPU_CLK_UNHALTED.REF_TSC / TSC</t>
+        </is>
+      </c>
+      <c r="H68" s="7" t="n"/>
+      <c r="I68" s="7" t="n"/>
+      <c r="J68" s="81" t="inlineStr">
+        <is>
+          <t>Average CPU Utilization</t>
         </is>
       </c>
       <c r="K68" s="8" t="inlineStr">
@@ -3810,28 +3842,28 @@
     <row r="69">
       <c r="A69" s="8" t="inlineStr">
         <is>
-          <t>Info.Frontend</t>
+          <t>Info.Memory</t>
         </is>
       </c>
       <c r="B69" s="8" t="inlineStr">
         <is>
-          <t>Inst_Miss_Cost_L3Hit_Percent</t>
+          <t>Cycles_per_Demand_Load_L2_Hit</t>
         </is>
       </c>
       <c r="C69" s="8" t="n"/>
       <c r="D69" s="8" t="n"/>
       <c r="E69" s="8" t="n"/>
-      <c r="F69" s="44" t="inlineStr">
-        <is>
-          <t>100 * MEM_BOUND_STALLS.IFETCH_LLC_HIT / ( MEM_BOUND_STALLS.IFETCH )</t>
-        </is>
-      </c>
-      <c r="G69" s="44" t="n"/>
-      <c r="H69" s="44" t="n"/>
-      <c r="I69" s="44" t="n"/>
+      <c r="F69" s="7" t="inlineStr">
+        <is>
+          <t>MEM_BOUND_STALLS.LOAD_L2_HIT / MEM_LOAD_UOPS_RETIRED.L2_HIT</t>
+        </is>
+      </c>
+      <c r="G69" s="7" t="n"/>
+      <c r="H69" s="7" t="n"/>
+      <c r="I69" s="7" t="n"/>
       <c r="J69" s="8" t="inlineStr">
         <is>
-          <t>Percent of instruction miss cost that hit in the L3</t>
+          <t>Cycle cost per L2 hit</t>
         </is>
       </c>
       <c r="K69" s="8" t="inlineStr">
@@ -3844,28 +3876,28 @@
     <row r="70">
       <c r="A70" s="8" t="inlineStr">
         <is>
-          <t>Info.Frontend</t>
+          <t>Info.Memory</t>
         </is>
       </c>
       <c r="B70" s="8" t="inlineStr">
         <is>
-          <t>Inst_Miss_Cost_DRAMHit_Percent</t>
+          <t>Cycles_per_Demand_Load_L3_Hit</t>
         </is>
       </c>
       <c r="C70" s="8" t="n"/>
       <c r="D70" s="8" t="n"/>
       <c r="E70" s="8" t="n"/>
-      <c r="F70" s="44" t="inlineStr">
-        <is>
-          <t>100 * MEM_BOUND_STALLS.IFETCH_DRAM_HIT / ( MEM_BOUND_STALLS.IFETCH )</t>
-        </is>
-      </c>
-      <c r="G70" s="44" t="n"/>
-      <c r="H70" s="44" t="n"/>
-      <c r="I70" s="44" t="n"/>
+      <c r="F70" s="7" t="inlineStr">
+        <is>
+          <t>MEM_BOUND_STALLS.LOAD_LLC_HIT / MEM_LOAD_UOPS_RETIRED.L3_HIT</t>
+        </is>
+      </c>
+      <c r="G70" s="7" t="n"/>
+      <c r="H70" s="7" t="n"/>
+      <c r="I70" s="7" t="n"/>
       <c r="J70" s="8" t="inlineStr">
         <is>
-          <t>Percent of instruction miss cost that hit in DRAM</t>
+          <t>Cycle cost per LLC hit</t>
         </is>
       </c>
       <c r="K70" s="8" t="inlineStr">
@@ -3883,27 +3915,23 @@
       </c>
       <c r="B71" s="8" t="inlineStr">
         <is>
-          <t>MemLoadPKI</t>
+          <t>Cycles_per_Demand_Load_DRAM_Hit</t>
         </is>
       </c>
       <c r="C71" s="8" t="n"/>
       <c r="D71" s="8" t="n"/>
       <c r="E71" s="8" t="n"/>
-      <c r="F71" s="44" t="inlineStr">
-        <is>
-          <t>1000 * MEM_UOPS_RETIRED.ALL_LOADS / INST_RETIRED.ANY</t>
-        </is>
-      </c>
-      <c r="G71" s="44" t="inlineStr">
-        <is>
-          <t>1000 * MEM_UOPS_RETIRED.ALL_LOADS / INST_RETIRED.ANY</t>
-        </is>
-      </c>
-      <c r="H71" s="44" t="n"/>
-      <c r="I71" s="44" t="n"/>
+      <c r="F71" s="7" t="inlineStr">
+        <is>
+          <t>MEM_BOUND_STALLS.LOAD_DRAM_HIT / MEM_LOAD_UOPS_RETIRED.DRAM_HIT</t>
+        </is>
+      </c>
+      <c r="G71" s="7" t="n"/>
+      <c r="H71" s="7" t="n"/>
+      <c r="I71" s="7" t="n"/>
       <c r="J71" s="8" t="inlineStr">
         <is>
-          <t>load ops retired per 1000 instruction</t>
+          <t>Cycle cost per DRAM hit</t>
         </is>
       </c>
       <c r="K71" s="8" t="inlineStr">
@@ -3916,32 +3944,28 @@
     <row r="72">
       <c r="A72" s="8" t="inlineStr">
         <is>
-          <t>Info.System</t>
-        </is>
-      </c>
-      <c r="B72" s="10" t="inlineStr">
-        <is>
-          <t>MUX</t>
+          <t>Info.Frontend</t>
+        </is>
+      </c>
+      <c r="B72" s="8" t="inlineStr">
+        <is>
+          <t>Inst_Miss_Cost_L2Hit_Percent</t>
         </is>
       </c>
       <c r="C72" s="8" t="n"/>
       <c r="D72" s="8" t="n"/>
       <c r="E72" s="8" t="n"/>
-      <c r="F72" s="44" t="inlineStr">
-        <is>
-          <t>CLKS_P / CLKS</t>
-        </is>
-      </c>
-      <c r="G72" s="44" t="inlineStr">
-        <is>
-          <t>CLKS_P / CLKS</t>
-        </is>
-      </c>
-      <c r="H72" s="44" t="n"/>
-      <c r="I72" s="44" t="n"/>
-      <c r="J72" s="11" t="inlineStr">
-        <is>
-          <t>PerfMon Event Multiplexing accuracy indicator</t>
+      <c r="F72" s="7" t="inlineStr">
+        <is>
+          <t>100 * MEM_BOUND_STALLS.IFETCH_L2_HIT / ( MEM_BOUND_STALLS.IFETCH )</t>
+        </is>
+      </c>
+      <c r="G72" s="7" t="n"/>
+      <c r="H72" s="7" t="n"/>
+      <c r="I72" s="7" t="n"/>
+      <c r="J72" s="8" t="inlineStr">
+        <is>
+          <t>Percent of instruction miss cost that hit in the L2</t>
         </is>
       </c>
       <c r="K72" s="8" t="inlineStr">
@@ -3949,27 +3973,35 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="L72" s="11" t="inlineStr">
-        <is>
-          <t>( &gt; 1.1 | &lt; 0.9 )</t>
-        </is>
-      </c>
+      <c r="L72" s="8" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="8" t="inlineStr">
         <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="B73" s="8" t="n"/>
+          <t>Info.Frontend</t>
+        </is>
+      </c>
+      <c r="B73" s="8" t="inlineStr">
+        <is>
+          <t>Inst_Miss_Cost_L3Hit_Percent</t>
+        </is>
+      </c>
       <c r="C73" s="8" t="n"/>
       <c r="D73" s="8" t="n"/>
       <c r="E73" s="8" t="n"/>
-      <c r="F73" s="44" t="n"/>
-      <c r="G73" s="44" t="n"/>
-      <c r="H73" s="44" t="n"/>
-      <c r="I73" s="44" t="n"/>
-      <c r="J73" s="8" t="n"/>
+      <c r="F73" s="7" t="inlineStr">
+        <is>
+          <t>100 * MEM_BOUND_STALLS.IFETCH_LLC_HIT / ( MEM_BOUND_STALLS.IFETCH )</t>
+        </is>
+      </c>
+      <c r="G73" s="7" t="n"/>
+      <c r="H73" s="7" t="n"/>
+      <c r="I73" s="7" t="n"/>
+      <c r="J73" s="8" t="inlineStr">
+        <is>
+          <t>Percent of instruction miss cost that hit in the L3</t>
+        </is>
+      </c>
       <c r="K73" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
@@ -3980,28 +4012,28 @@
     <row r="74">
       <c r="A74" s="8" t="inlineStr">
         <is>
-          <t>Aux</t>
+          <t>Info.Frontend</t>
         </is>
       </c>
       <c r="B74" s="8" t="inlineStr">
         <is>
-          <t>#Pipeline_Width</t>
+          <t>Inst_Miss_Cost_DRAMHit_Percent</t>
         </is>
       </c>
       <c r="C74" s="8" t="n"/>
       <c r="D74" s="8" t="n"/>
       <c r="E74" s="8" t="n"/>
-      <c r="F74" s="44" t="n">
-        <v>4</v>
-      </c>
-      <c r="G74" s="44" t="n">
-        <v>3</v>
-      </c>
-      <c r="H74" s="44" t="n"/>
-      <c r="I74" s="44" t="n"/>
+      <c r="F74" s="7" t="inlineStr">
+        <is>
+          <t>100 * MEM_BOUND_STALLS.IFETCH_DRAM_HIT / ( MEM_BOUND_STALLS.IFETCH )</t>
+        </is>
+      </c>
+      <c r="G74" s="7" t="n"/>
+      <c r="H74" s="7" t="n"/>
+      <c r="I74" s="7" t="n"/>
       <c r="J74" s="8" t="inlineStr">
         <is>
-          <t>pipeline allocation width</t>
+          <t>Percent of instruction miss cost that hit in DRAM</t>
         </is>
       </c>
       <c r="K74" s="8" t="inlineStr">
@@ -4014,17 +4046,141 @@
     <row r="75">
       <c r="A75" s="8" t="inlineStr">
         <is>
+          <t>Info.Memory</t>
+        </is>
+      </c>
+      <c r="B75" s="8" t="inlineStr">
+        <is>
+          <t>MemLoadPKI</t>
+        </is>
+      </c>
+      <c r="C75" s="8" t="n"/>
+      <c r="D75" s="8" t="n"/>
+      <c r="E75" s="8" t="n"/>
+      <c r="F75" s="7" t="inlineStr">
+        <is>
+          <t>1000 * MEM_UOPS_RETIRED.ALL_LOADS / INST_RETIRED.ANY</t>
+        </is>
+      </c>
+      <c r="G75" s="7" t="inlineStr">
+        <is>
+          <t>1000 * MEM_UOPS_RETIRED.ALL_LOADS / INST_RETIRED.ANY</t>
+        </is>
+      </c>
+      <c r="H75" s="7" t="n"/>
+      <c r="I75" s="7" t="n"/>
+      <c r="J75" s="8" t="inlineStr">
+        <is>
+          <t>load ops retired per 1000 instruction</t>
+        </is>
+      </c>
+      <c r="K75" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L75" s="8" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="8" t="inlineStr">
+        <is>
+          <t>Info.System</t>
+        </is>
+      </c>
+      <c r="B76" s="10" t="inlineStr">
+        <is>
+          <t>MUX</t>
+        </is>
+      </c>
+      <c r="C76" s="8" t="n"/>
+      <c r="D76" s="8" t="n"/>
+      <c r="E76" s="8" t="n"/>
+      <c r="F76" s="7" t="inlineStr">
+        <is>
+          <t>CLKS_P / CLKS</t>
+        </is>
+      </c>
+      <c r="G76" s="7" t="inlineStr">
+        <is>
+          <t>CLKS_P / CLKS</t>
+        </is>
+      </c>
+      <c r="H76" s="7" t="n"/>
+      <c r="I76" s="7" t="n"/>
+      <c r="J76" s="11" t="inlineStr">
+        <is>
+          <t>PerfMon Event Multiplexing accuracy indicator</t>
+        </is>
+      </c>
+      <c r="K76" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L76" s="11" t="inlineStr">
+        <is>
+          <t>( &gt; 1.1 | &lt; 0.9 )</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="8" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="B77" s="8" t="n"/>
+      <c r="C77" s="8" t="n"/>
+      <c r="D77" s="8" t="n"/>
+      <c r="E77" s="8" t="n"/>
+      <c r="F77" s="7" t="n"/>
+      <c r="G77" s="7" t="n"/>
+      <c r="H77" s="7" t="n"/>
+      <c r="I77" s="7" t="n"/>
+      <c r="J77" s="8" t="n"/>
+      <c r="K77" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L77" s="8" t="n"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="8" t="inlineStr">
+        <is>
           <t>Aux</t>
         </is>
       </c>
-      <c r="B75" s="8" t="inlineStr">
-        <is>
-          <t>MEM_BOUND_STALLS_AT_RET_CORRECTION</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" s="8" t="n"/>
+      <c r="B78" s="8" t="inlineStr">
+        <is>
+          <t>#Pipeline_Width</t>
+        </is>
+      </c>
+      <c r="C78" s="8" t="n"/>
+      <c r="D78" s="8" t="n"/>
+      <c r="E78" s="8" t="n"/>
+      <c r="F78" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G78" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H78" s="7" t="n"/>
+      <c r="I78" s="7" t="n"/>
+      <c r="J78" s="8" t="inlineStr">
+        <is>
+          <t>pipeline allocation width</t>
+        </is>
+      </c>
+      <c r="K78" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L78" s="8" t="n"/>
+    </row>
+    <row r="79">
+      <c r="B79" s="8" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4037,7 +4193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4050,32 +4206,45 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="inlineStr">
+      <c r="A1" s="42" t="inlineStr">
         <is>
           <t>Version</t>
         </is>
       </c>
-      <c r="B1" s="46" t="inlineStr">
+      <c r="B1" s="43" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
       </c>
-      <c r="C1" s="47" t="inlineStr">
+      <c r="C1" s="44" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53" t="n">
+      <c r="A2" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B2" s="82" t="inlineStr">
+        <is>
+          <t>FP_UOPS changed to FPDIV_Uops, Added BR_MISP breakdown stats; Frontend_Bandwidth/Latency changed to Fetch_Bandwidth/Latency; Load_Store_Bound changed to Memory_Bound; Icache changed to ICache_Misses; ITLB changed to ITLB_Misses</t>
+        </is>
+      </c>
+      <c r="C2" s="83" t="n">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="84" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Initial Release</t>
         </is>
       </c>
-      <c r="C2" s="79" t="n">
+      <c r="C3" s="83" t="n">
         <v>44789</v>
       </c>
     </row>

</xml_diff>

<commit_message>
E-core TMA update 3.51 Atom TMA update 1.2
Signed-off-by: Ryan P Mclaughlin <ryan.p.mclaughlin@intel.com>
</commit_message>
<xml_diff>
--- a/Atom_TMA.xlsx
+++ b/Atom_TMA.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="575" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" tabRatio="575" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Change Log" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -240,6 +240,13 @@
       <name val="-apple-system"/>
       <color theme="1"/>
       <sz val="10.5"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="54">
@@ -805,7 +812,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -898,6 +905,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="34" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -928,10 +936,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="43">
@@ -979,7 +987,20 @@
     <cellStyle name="60% - Accent6" xfId="41" builtinId="52"/>
     <cellStyle name="Normal 2 2" xfId="42"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1300,7 +1321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1320,7 +1341,7 @@
         </is>
       </c>
       <c r="C1" s="3" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="2">
@@ -1331,62 +1352,62 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="58" t="inlineStr">
+      <c r="A3" s="59" t="inlineStr">
         <is>
           <t>Key</t>
         </is>
       </c>
-      <c r="B3" s="58" t="inlineStr">
+      <c r="B3" s="59" t="inlineStr">
         <is>
           <t>Level1</t>
         </is>
       </c>
-      <c r="C3" s="58" t="inlineStr">
+      <c r="C3" s="59" t="inlineStr">
         <is>
           <t>Level2</t>
         </is>
       </c>
-      <c r="D3" s="58" t="inlineStr">
+      <c r="D3" s="59" t="inlineStr">
         <is>
           <t>Level3</t>
         </is>
       </c>
-      <c r="E3" s="58" t="inlineStr">
+      <c r="E3" s="59" t="inlineStr">
         <is>
           <t>Level4</t>
         </is>
       </c>
-      <c r="F3" s="58" t="inlineStr">
+      <c r="F3" s="59" t="inlineStr">
         <is>
           <t>TNT</t>
         </is>
       </c>
-      <c r="G3" s="58" t="inlineStr">
+      <c r="G3" s="59" t="inlineStr">
         <is>
           <t>GLM/GLP</t>
         </is>
       </c>
-      <c r="H3" s="58" t="inlineStr">
+      <c r="H3" s="59" t="inlineStr">
         <is>
           <t>Locate-with</t>
         </is>
       </c>
-      <c r="I3" s="58" t="inlineStr">
+      <c r="I3" s="59" t="inlineStr">
         <is>
           <t>Count Domain</t>
         </is>
       </c>
-      <c r="J3" s="58" t="inlineStr">
+      <c r="J3" s="59" t="inlineStr">
         <is>
           <t>Metric Description</t>
         </is>
       </c>
-      <c r="K3" s="58" t="inlineStr">
+      <c r="K3" s="59" t="inlineStr">
         <is>
           <t>Metric Group</t>
         </is>
       </c>
-      <c r="L3" s="58" t="inlineStr">
+      <c r="L3" s="59" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
@@ -1398,7 +1419,7 @@
           <t>FE</t>
         </is>
       </c>
-      <c r="B4" s="59" t="inlineStr">
+      <c r="B4" s="60" t="inlineStr">
         <is>
           <t>Frontend_Bound</t>
         </is>
@@ -1441,7 +1462,7 @@
         </is>
       </c>
       <c r="B5" s="24" t="n"/>
-      <c r="C5" s="60" t="inlineStr">
+      <c r="C5" s="61" t="inlineStr">
         <is>
           <t>Fetch_Latency</t>
         </is>
@@ -1480,7 +1501,7 @@
       </c>
       <c r="B6" s="24" t="n"/>
       <c r="C6" s="24" t="n"/>
-      <c r="D6" s="61" t="inlineStr">
+      <c r="D6" s="62" t="inlineStr">
         <is>
           <t>ICache_Misses</t>
         </is>
@@ -1518,7 +1539,7 @@
       </c>
       <c r="B7" s="24" t="n"/>
       <c r="C7" s="24" t="n"/>
-      <c r="D7" s="61" t="inlineStr">
+      <c r="D7" s="62" t="inlineStr">
         <is>
           <t>ITLB_Misses</t>
         </is>
@@ -1556,7 +1577,7 @@
       </c>
       <c r="B8" s="24" t="n"/>
       <c r="C8" s="24" t="n"/>
-      <c r="D8" s="61" t="inlineStr">
+      <c r="D8" s="62" t="inlineStr">
         <is>
           <t>Branch_Detect</t>
         </is>
@@ -1594,7 +1615,7 @@
       </c>
       <c r="B9" s="24" t="n"/>
       <c r="C9" s="24" t="n"/>
-      <c r="D9" s="61" t="inlineStr">
+      <c r="D9" s="62" t="inlineStr">
         <is>
           <t>Branch_Resteer</t>
         </is>
@@ -1631,7 +1652,7 @@
         </is>
       </c>
       <c r="B10" s="24" t="n"/>
-      <c r="C10" s="60" t="inlineStr">
+      <c r="C10" s="61" t="inlineStr">
         <is>
           <t>Fetch_Bandwidth</t>
         </is>
@@ -1670,7 +1691,7 @@
       </c>
       <c r="B11" s="24" t="n"/>
       <c r="C11" s="24" t="n"/>
-      <c r="D11" s="61" t="inlineStr">
+      <c r="D11" s="62" t="inlineStr">
         <is>
           <t>Cisc</t>
         </is>
@@ -1708,7 +1729,7 @@
       </c>
       <c r="B12" s="24" t="n"/>
       <c r="C12" s="24" t="n"/>
-      <c r="D12" s="61" t="inlineStr">
+      <c r="D12" s="62" t="inlineStr">
         <is>
           <t>Decode</t>
         </is>
@@ -1746,7 +1767,7 @@
       </c>
       <c r="B13" s="24" t="n"/>
       <c r="C13" s="24" t="n"/>
-      <c r="D13" s="61" t="inlineStr">
+      <c r="D13" s="62" t="inlineStr">
         <is>
           <t>Predecode</t>
         </is>
@@ -1784,7 +1805,7 @@
       </c>
       <c r="B14" s="24" t="n"/>
       <c r="C14" s="24" t="n"/>
-      <c r="D14" s="61" t="inlineStr">
+      <c r="D14" s="62" t="inlineStr">
         <is>
           <t>Other_FB</t>
         </is>
@@ -1820,13 +1841,13 @@
           <t>BAD</t>
         </is>
       </c>
-      <c r="B15" s="62" t="inlineStr">
+      <c r="B15" s="63" t="inlineStr">
         <is>
           <t>Bad_Speculation</t>
         </is>
       </c>
-      <c r="C15" s="63" t="n"/>
-      <c r="D15" s="63" t="n"/>
+      <c r="C15" s="64" t="n"/>
+      <c r="D15" s="64" t="n"/>
       <c r="E15" s="8" t="n"/>
       <c r="F15" s="7" t="inlineStr">
         <is>
@@ -1862,13 +1883,13 @@
           <t>BAD</t>
         </is>
       </c>
-      <c r="B16" s="63" t="n"/>
-      <c r="C16" s="64" t="inlineStr">
+      <c r="B16" s="64" t="n"/>
+      <c r="C16" s="65" t="inlineStr">
         <is>
           <t>Branch_Mispredicts</t>
         </is>
       </c>
-      <c r="D16" s="63" t="n"/>
+      <c r="D16" s="64" t="n"/>
       <c r="E16" s="8" t="n"/>
       <c r="F16" s="7" t="inlineStr">
         <is>
@@ -1900,13 +1921,13 @@
           <t>BAD</t>
         </is>
       </c>
-      <c r="B17" s="65" t="n"/>
-      <c r="C17" s="64" t="inlineStr">
+      <c r="B17" s="66" t="n"/>
+      <c r="C17" s="65" t="inlineStr">
         <is>
           <t>Machine_Clears</t>
         </is>
       </c>
-      <c r="D17" s="63" t="n"/>
+      <c r="D17" s="64" t="n"/>
       <c r="E17" s="8" t="n"/>
       <c r="F17" s="7" t="inlineStr">
         <is>
@@ -1938,9 +1959,9 @@
           <t>BAD</t>
         </is>
       </c>
-      <c r="B18" s="63" t="n"/>
-      <c r="C18" s="63" t="n"/>
-      <c r="D18" s="66" t="inlineStr">
+      <c r="B18" s="64" t="n"/>
+      <c r="C18" s="64" t="n"/>
+      <c r="D18" s="67" t="inlineStr">
         <is>
           <t>Fast_Nuke</t>
         </is>
@@ -1976,7 +1997,7 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B19" s="67" t="inlineStr">
+      <c r="B19" s="68" t="inlineStr">
         <is>
           <t>Backend_Bound</t>
         </is>
@@ -2018,8 +2039,8 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B20" s="68" t="n"/>
-      <c r="C20" s="69" t="inlineStr">
+      <c r="B20" s="69" t="n"/>
+      <c r="C20" s="70" t="inlineStr">
         <is>
           <t>Core_Bound</t>
         </is>
@@ -2039,7 +2060,7 @@
       </c>
       <c r="J20" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Counts the number of cycles due to backend bound stalls that are core execution bound and not attributed to outstanding demand load or store stalls. </t>
+          <t>Counts the number of cycles due to backend bound stalls that are core execution bound and not attributed to outstanding demand load or store stalls.</t>
         </is>
       </c>
       <c r="K20" s="8" t="n"/>
@@ -2055,8 +2076,8 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B21" s="68" t="n"/>
-      <c r="C21" s="69" t="inlineStr">
+      <c r="B21" s="69" t="n"/>
+      <c r="C21" s="70" t="inlineStr">
         <is>
           <t>Memory_Bound</t>
         </is>
@@ -2077,7 +2098,7 @@
       </c>
       <c r="J21" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Counts the number of cycles the core is stalled due to stores or loads. </t>
+          <t>Counts the number of cycles the core is stalled due to stores or loads.</t>
         </is>
       </c>
       <c r="K21" s="8" t="n"/>
@@ -2095,7 +2116,7 @@
       </c>
       <c r="B22" s="57" t="n"/>
       <c r="C22" s="57" t="n"/>
-      <c r="D22" s="70" t="inlineStr">
+      <c r="D22" s="71" t="inlineStr">
         <is>
           <t>Store_Bound</t>
         </is>
@@ -2131,8 +2152,8 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="B23" s="65" t="n"/>
-      <c r="D23" s="71" t="inlineStr">
+      <c r="B23" s="66" t="n"/>
+      <c r="D23" s="72" t="inlineStr">
         <is>
           <t>L2_Bound</t>
         </is>
@@ -2168,7 +2189,7 @@
         </is>
       </c>
       <c r="B24" s="57" t="n"/>
-      <c r="D24" s="71" t="inlineStr">
+      <c r="D24" s="72" t="inlineStr">
         <is>
           <t>L3_Bound</t>
         </is>
@@ -2239,13 +2260,13 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B26" s="72" t="inlineStr">
+      <c r="B26" s="73" t="inlineStr">
         <is>
           <t>Backend_Bound_Aux</t>
         </is>
       </c>
-      <c r="C26" s="63" t="n"/>
-      <c r="D26" s="63" t="n"/>
+      <c r="C26" s="64" t="n"/>
+      <c r="D26" s="64" t="n"/>
       <c r="E26" s="8" t="n"/>
       <c r="F26" s="7" t="inlineStr">
         <is>
@@ -2265,7 +2286,7 @@
       </c>
       <c r="J26" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Counts the total number of issue slots  that were not consumed by the backend due to backend stalls.  Note that UOPS must be available for consumption in order for this event to count.  If a uop is not available (IQ is empty), this event will not count.  All of these subevents count backend stalls, in slots, due to a resource limitation.   These are not cycle based events and therefore can not be precisely added or subtracted from the Backend_Bound subevents which are cycle based.  These subevents are supplementary to Backend_Bound and can be used to analyze results from a resource perspective at allocation.  </t>
+          <t>Counts the total number of issue slots  that were not consumed by the backend due to backend stalls.  Note that UOPS must be available for consumption in order for this event to count.  If a uop is not available (IQ is empty), this event will not count.  All of these subevents count backend stalls, in slots, due to a resource limitation.   These are not cycle based events and therefore can not be precisely added or subtracted from the Backend_Bound subevents which are cycle based.  These subevents are supplementary to Backend_Bound and can be used to analyze results from a resource perspective at allocation.</t>
         </is>
       </c>
       <c r="K26" s="8" t="n"/>
@@ -2281,13 +2302,13 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B27" s="63" t="n"/>
-      <c r="C27" s="73" t="inlineStr">
+      <c r="B27" s="64" t="n"/>
+      <c r="C27" s="74" t="inlineStr">
         <is>
           <t>Resource_Bound</t>
         </is>
       </c>
-      <c r="D27" s="63" t="n"/>
+      <c r="D27" s="64" t="n"/>
       <c r="E27" s="8" t="n"/>
       <c r="F27" s="7" t="inlineStr">
         <is>
@@ -2303,7 +2324,7 @@
       </c>
       <c r="J27" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Counts the total number of issue slots  that were not consumed by the backend due to backend stalls.  Note that uops must be available for consumption in order for this event to count.  If a uop is not available (IQ is empty), this event will not count. </t>
+          <t>Counts the total number of issue slots  that were not consumed by the backend due to backend stalls.  Note that uops must be available for consumption in order for this event to count.  If a uop is not available (IQ is empty), this event will not count.</t>
         </is>
       </c>
       <c r="K27" s="8" t="n"/>
@@ -2319,9 +2340,9 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B28" s="63" t="n"/>
-      <c r="C28" s="63" t="n"/>
-      <c r="D28" s="74" t="inlineStr">
+      <c r="B28" s="64" t="n"/>
+      <c r="C28" s="64" t="n"/>
+      <c r="D28" s="75" t="inlineStr">
         <is>
           <t>Mem_Scheduler</t>
         </is>
@@ -2357,9 +2378,9 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B29" s="63" t="n"/>
-      <c r="C29" s="63" t="n"/>
-      <c r="D29" s="74" t="inlineStr">
+      <c r="B29" s="64" t="n"/>
+      <c r="C29" s="64" t="n"/>
+      <c r="D29" s="75" t="inlineStr">
         <is>
           <t>Non_Mem_Scheduler</t>
         </is>
@@ -2395,9 +2416,9 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B30" s="63" t="n"/>
-      <c r="C30" s="63" t="n"/>
-      <c r="D30" s="74" t="inlineStr">
+      <c r="B30" s="64" t="n"/>
+      <c r="C30" s="64" t="n"/>
+      <c r="D30" s="75" t="inlineStr">
         <is>
           <t>Register</t>
         </is>
@@ -2433,9 +2454,9 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B31" s="63" t="n"/>
-      <c r="C31" s="63" t="n"/>
-      <c r="D31" s="74" t="inlineStr">
+      <c r="B31" s="64" t="n"/>
+      <c r="C31" s="64" t="n"/>
+      <c r="D31" s="75" t="inlineStr">
         <is>
           <t>Reorder_Buffer</t>
         </is>
@@ -2471,9 +2492,9 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B32" s="63" t="n"/>
-      <c r="C32" s="63" t="n"/>
-      <c r="D32" s="74" t="inlineStr">
+      <c r="B32" s="64" t="n"/>
+      <c r="C32" s="64" t="n"/>
+      <c r="D32" s="75" t="inlineStr">
         <is>
           <t>Store_Buffer</t>
         </is>
@@ -2509,9 +2530,9 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B33" s="63" t="n"/>
-      <c r="C33" s="63" t="n"/>
-      <c r="D33" s="74" t="inlineStr">
+      <c r="B33" s="64" t="n"/>
+      <c r="C33" s="64" t="n"/>
+      <c r="D33" s="75" t="inlineStr">
         <is>
           <t>Alloc_Restriction</t>
         </is>
@@ -2547,9 +2568,9 @@
           <t>BE_aux</t>
         </is>
       </c>
-      <c r="B34" s="63" t="n"/>
-      <c r="C34" s="63" t="n"/>
-      <c r="D34" s="74" t="inlineStr">
+      <c r="B34" s="64" t="n"/>
+      <c r="C34" s="64" t="n"/>
+      <c r="D34" s="75" t="inlineStr">
         <is>
           <t>Serialization</t>
         </is>
@@ -2585,7 +2606,7 @@
           <t>RET</t>
         </is>
       </c>
-      <c r="B35" s="75" t="inlineStr">
+      <c r="B35" s="76" t="inlineStr">
         <is>
           <t>Retiring</t>
         </is>
@@ -2611,7 +2632,7 @@
       </c>
       <c r="J35" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Counts the numer of issue slots  that result in retirement slots. </t>
+          <t>Counts the number of issue slots  that result in retirement slots.</t>
         </is>
       </c>
       <c r="K35" s="8" t="n"/>
@@ -2627,8 +2648,8 @@
           <t>RET</t>
         </is>
       </c>
-      <c r="B36" s="63" t="n"/>
-      <c r="C36" s="76" t="inlineStr">
+      <c r="B36" s="64" t="n"/>
+      <c r="C36" s="77" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
@@ -2649,7 +2670,7 @@
       </c>
       <c r="J36" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Counts the number of uops that are not from the microsequencer. </t>
+          <t>Counts the number of uops that are not from the microsequencer.</t>
         </is>
       </c>
       <c r="K36" s="8" t="n"/>
@@ -2665,9 +2686,9 @@
           <t>RET</t>
         </is>
       </c>
-      <c r="B37" s="63" t="n"/>
+      <c r="B37" s="64" t="n"/>
       <c r="C37" s="57" t="n"/>
-      <c r="D37" s="77" t="inlineStr">
+      <c r="D37" s="78" t="inlineStr">
         <is>
           <t>FPDIV_uops</t>
         </is>
@@ -2707,9 +2728,9 @@
           <t>RET</t>
         </is>
       </c>
-      <c r="B38" s="63" t="n"/>
+      <c r="B38" s="64" t="n"/>
       <c r="C38" s="57" t="n"/>
-      <c r="D38" s="77" t="inlineStr">
+      <c r="D38" s="78" t="inlineStr">
         <is>
           <t>Other_Ret</t>
         </is>
@@ -2740,42 +2761,42 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="78" t="inlineStr">
+      <c r="A39" s="79" t="inlineStr">
         <is>
           <t>RET</t>
         </is>
       </c>
-      <c r="B39" s="78" t="n"/>
-      <c r="C39" s="79" t="inlineStr">
+      <c r="B39" s="79" t="n"/>
+      <c r="C39" s="80" t="inlineStr">
         <is>
           <t>MS_uops</t>
         </is>
       </c>
-      <c r="D39" s="78" t="n"/>
-      <c r="E39" s="78" t="n"/>
-      <c r="F39" s="80" t="inlineStr">
+      <c r="D39" s="79" t="n"/>
+      <c r="E39" s="79" t="n"/>
+      <c r="F39" s="81" t="inlineStr">
         <is>
           <t>UOPS_RETIRED.MS / SLOTS</t>
         </is>
       </c>
-      <c r="G39" s="80" t="inlineStr">
+      <c r="G39" s="81" t="inlineStr">
         <is>
           <t>UOPS_RETIRED.MS / SLOTS</t>
         </is>
       </c>
-      <c r="H39" s="80" t="n"/>
-      <c r="I39" s="80" t="inlineStr">
+      <c r="H39" s="81" t="n"/>
+      <c r="I39" s="81" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
       </c>
-      <c r="J39" s="78" t="inlineStr">
+      <c r="J39" s="79" t="inlineStr">
         <is>
           <t>Counts the number of uops that are from the complex flows issued by the micro-sequencer (MS).  This includes uops from flows due to complex instructions, faults, assists, and inserted flows.</t>
         </is>
       </c>
       <c r="K39" s="19" t="n"/>
-      <c r="L39" s="78" t="inlineStr">
+      <c r="L39" s="79" t="inlineStr">
         <is>
           <t>&gt;0.05</t>
         </is>
@@ -2802,7 +2823,7 @@
       <c r="J40" s="8" t="n"/>
       <c r="K40" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L40" s="8" t="n"/>
@@ -2840,7 +2861,7 @@
       <c r="J41" s="8" t="n"/>
       <c r="K41" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L41" s="8" t="n"/>
@@ -2878,7 +2899,7 @@
       <c r="J42" s="8" t="n"/>
       <c r="K42" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L42" s="8" t="n"/>
@@ -2916,7 +2937,7 @@
       <c r="J43" s="8" t="n"/>
       <c r="K43" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L43" s="8" t="n"/>
@@ -2954,7 +2975,7 @@
       </c>
       <c r="K44" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L44" s="8" t="n"/>
@@ -2992,7 +3013,7 @@
       </c>
       <c r="K45" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L45" s="8" t="n"/>
@@ -3030,7 +3051,7 @@
       </c>
       <c r="K46" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L46" s="8" t="n"/>
@@ -3165,12 +3186,12 @@
       <c r="I50" s="7" t="n"/>
       <c r="J50" s="8" t="inlineStr">
         <is>
-          <t>Instructions per Branch (lower number means higher occurance rate)</t>
+          <t>Instructions per Branch (lower number means higher occurence rate)</t>
         </is>
       </c>
       <c r="K50" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L50" s="8" t="n"/>
@@ -3203,12 +3224,12 @@
       <c r="I51" s="7" t="n"/>
       <c r="J51" s="8" t="inlineStr">
         <is>
-          <t>Instruction per (near) call (lower number means higher occurance rate)</t>
+          <t>Instruction per (near) call (lower number means higher occurence rate)</t>
         </is>
       </c>
       <c r="K51" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L51" s="8" t="n"/>
@@ -3246,7 +3267,7 @@
       </c>
       <c r="K52" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L52" s="8" t="n"/>
@@ -3284,7 +3305,7 @@
       </c>
       <c r="K53" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L53" s="8" t="n"/>
@@ -3322,7 +3343,7 @@
       </c>
       <c r="K54" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L54" s="8" t="n"/>
@@ -3496,7 +3517,7 @@
       </c>
       <c r="K59" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L59" s="8" t="n"/>
@@ -3534,7 +3555,7 @@
       </c>
       <c r="K60" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L60" s="8" t="n"/>
@@ -3572,7 +3593,7 @@
       </c>
       <c r="K61" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L61" s="8" t="n"/>
@@ -3610,7 +3631,7 @@
       </c>
       <c r="K62" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L62" s="8" t="n"/>
@@ -3648,7 +3669,7 @@
       </c>
       <c r="K63" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L63" s="8" t="n"/>
@@ -3686,7 +3707,7 @@
       </c>
       <c r="K64" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L64" s="8" t="n"/>
@@ -3720,7 +3741,7 @@
       </c>
       <c r="K65" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L65" s="8" t="n"/>
@@ -3758,7 +3779,7 @@
       </c>
       <c r="K66" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L66" s="8" t="n"/>
@@ -3796,7 +3817,7 @@
       </c>
       <c r="K67" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L67" s="8" t="n"/>
@@ -3827,14 +3848,14 @@
       </c>
       <c r="H68" s="7" t="n"/>
       <c r="I68" s="7" t="n"/>
-      <c r="J68" s="81" t="inlineStr">
+      <c r="J68" s="82" t="inlineStr">
         <is>
           <t>Average CPU Utilization</t>
         </is>
       </c>
       <c r="K68" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L68" s="8" t="n"/>
@@ -3868,7 +3889,7 @@
       </c>
       <c r="K69" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L69" s="8" t="n"/>
@@ -3902,7 +3923,7 @@
       </c>
       <c r="K70" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L70" s="8" t="n"/>
@@ -3936,7 +3957,7 @@
       </c>
       <c r="K71" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L71" s="8" t="n"/>
@@ -3970,7 +3991,7 @@
       </c>
       <c r="K72" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L72" s="8" t="n"/>
@@ -4004,7 +4025,7 @@
       </c>
       <c r="K73" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L73" s="8" t="n"/>
@@ -4038,7 +4059,7 @@
       </c>
       <c r="K74" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L74" s="8" t="n"/>
@@ -4076,7 +4097,7 @@
       </c>
       <c r="K75" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L75" s="8" t="n"/>
@@ -4114,7 +4135,7 @@
       </c>
       <c r="K76" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L76" s="11" t="inlineStr">
@@ -4140,7 +4161,7 @@
       <c r="J77" s="8" t="n"/>
       <c r="K77" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L77" s="8" t="n"/>
@@ -4174,13 +4195,10 @@
       </c>
       <c r="K78" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="L78" s="8" t="n"/>
-    </row>
-    <row r="79">
-      <c r="B79" s="8" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4193,7 +4211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4224,27 +4242,40 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Spelling fixes for occurrence, number; Removed trailing spaces on several descriptions</t>
+        </is>
+      </c>
+      <c r="C2" s="83" t="n">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1.1</v>
       </c>
-      <c r="B2" s="82" t="inlineStr">
+      <c r="B3" s="84" t="inlineStr">
         <is>
           <t>FP_UOPS changed to FPDIV_Uops, Added BR_MISP breakdown stats; Frontend_Bandwidth/Latency changed to Fetch_Bandwidth/Latency; Load_Store_Bound changed to Memory_Bound; Icache changed to ICache_Misses; ITLB changed to ITLB_Misses</t>
         </is>
       </c>
-      <c r="C2" s="83" t="n">
+      <c r="C3" s="83" t="n">
         <v>45013</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="84" t="n">
+    <row r="4">
+      <c r="A4" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Initial Release</t>
         </is>
       </c>
-      <c r="C3" s="83" t="n">
+      <c r="C4" s="83" t="n">
         <v>44789</v>
       </c>
     </row>

</xml_diff>